<commit_message>
checkpoint cleaning up vcr
</commit_message>
<xml_diff>
--- a/src/reports/_XL_Template.xlsx
+++ b/src/reports/_XL_Template.xlsx
@@ -536,10 +536,10 @@
     <col width="10" customWidth="1" min="4" max="4"/>
     <col width="7" customWidth="1" min="5" max="5"/>
     <col width="21" customWidth="1" min="6" max="6"/>
-    <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="23" customWidth="1" min="7" max="7"/>
     <col width="25" customWidth="1" min="8" max="8"/>
-    <col width="138" customWidth="1" min="9" max="9"/>
-    <col width="63" customWidth="1" min="10" max="10"/>
+    <col width="223" customWidth="1" min="9" max="9"/>
+    <col width="104" customWidth="1" min="10" max="10"/>
     <col width="25" customWidth="1" style="4" min="11" max="16384"/>
   </cols>
   <sheetData>
@@ -621,26 +621,30 @@
         <v>30</v>
       </c>
       <c r="F3" t="n">
-        <v>246166.0913371695</v>
+        <v>383607.4385447975</v>
       </c>
       <c r="G3" t="n">
-        <v>82974171407.47113</v>
+        <v>217189118922.9461</v>
       </c>
       <c r="H3" t="n">
-        <v>288052.3761531418</v>
+        <v>466035.5339702608</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>0: [-219.21688054714895, -283.4010412804356]
-1: [-263.1329501200152, -551.0857452447497]
-2: [-1009.0166192423145, -963.8000344970591]</t>
+          <t>0: [-493.8128470122012, -242.99050438298616]
+1: [63.1234238519379, 569.6521591978558]
+2: [-619.192099340552, 211.51338182575842]
+3: [-691.7730730065327, 416.09470660316936]
+4: [0.5997833923998921, 0.1317590904502821]</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>0: -423.879122823655
-1: -576.345784836871
-2: 1340.28332884399</t>
+          <t>0: -677.585800924159
+1: 432.58222739927
+2: 837.350506660305
+3: 1150.94701435421
+4: 603.512708136689</t>
         </is>
       </c>
     </row>
@@ -663,26 +667,30 @@
         <v>30</v>
       </c>
       <c r="F4" t="n">
-        <v>240542.9956853748</v>
+        <v>189548833.6473231</v>
       </c>
       <c r="G4" t="n">
-        <v>80217973746.73207</v>
+        <v>8.363999803312931e+16</v>
       </c>
       <c r="H4" t="n">
-        <v>283227.7771454136</v>
+        <v>289205805.6698194</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>0: [-1710.1405706336031, -2007.2292764013132]
-1: [-1623.7114116988444, -2245.2659923794504]
-2: [-3031.869504675193, -2725.58955367705]</t>
+          <t>0: [49.37034989377935, 165.04734797835474]
+1: [-202.13673421702197, 482.6491505048583]
+2: [-600.1111530018668, 317.5292516732453]
+3: [-468.71236811275065, 430.81849351972704]
+4: [23.600977763367794, 37.64692730341057]</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>0: -2503.3624211782
-1: -2612.54927490723
-2: 3826.83466699293</t>
+          <t>0: -435.276496585396
+1: 285.69928870636
+2: 905.312953142388
+3: 1016.59020982434
+4: 708.485990413814</t>
         </is>
       </c>
     </row>
@@ -705,26 +713,30 @@
         <v>30</v>
       </c>
       <c r="F5" t="n">
-        <v>234384.1505247882</v>
+        <v>898805.5897734326</v>
       </c>
       <c r="G5" t="n">
-        <v>77291275920.24577</v>
+        <v>2819031287465.641</v>
       </c>
       <c r="H5" t="n">
-        <v>278013.0858795064</v>
+        <v>1678997.107640642</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>0: [-3012.4500198326905, -3927.021865137133]
-1: [-2753.3412127622078, -3919.810292032463]
-2: [-5154.682718516888, -4442.270343653525]</t>
+          <t>0: [2.578198563199899, 151.20497640293067]
+1: [-233.07608948993072, 471.26616671780477]
+2: [-596.3531919504596, 317.0241042857275]
+3: [-456.54248691351194, 430.00524897328]
+4: [16.549044132375403, 36.408410133752824]</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>0: -4673.26133510884
-1: -4575.57165725912
-2: 6040.5282286018</t>
+          <t>0: -595.950346094813
+1: 278.987998999827
+2: 900.140788742676
+3: 1005.37956935888
+4: 688.082317612012</t>
         </is>
       </c>
     </row>
@@ -747,26 +759,30 @@
         <v>30</v>
       </c>
       <c r="F6" t="n">
-        <v>228360.1405089266</v>
+        <v>682280.7140842717</v>
       </c>
       <c r="G6" t="n">
-        <v>74505974570.19653</v>
+        <v>1568029813158.364</v>
       </c>
       <c r="H6" t="n">
-        <v>272957.8256254921</v>
+        <v>1252209.971673426</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>0: [-4074.0506504712193, -5382.004656886309]
-1: [-4106.005753682643, -5146.514973365565]
-2: [-7288.387422290418, -6114.829966521641]</t>
+          <t>0: [-25.19553677988207, 148.2821071642695]
+1: [-259.8357776976272, 459.9769054852552]
+2: [-597.7905433678027, 317.01501257444]
+3: [-455.69273799354863, 428.19116416032375]
+4: [16.48549622834818, 35.37604223588879]</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>0: -6770.8470159323
-1: -6880.04390664002
-2: 8288.63191474556</t>
+          <t>0: -695.715163481179
+1: 190.848312367366
+2: 940.489303947944
+3: 1037.71373737694
+4: 2027.0838702617</t>
         </is>
       </c>
     </row>
@@ -789,26 +805,30 @@
         <v>30</v>
       </c>
       <c r="F7" t="n">
-        <v>222449.4637596655</v>
+        <v>702698.7812704828</v>
       </c>
       <c r="G7" t="n">
-        <v>71845159299.22202</v>
+        <v>2001543778113.333</v>
       </c>
       <c r="H7" t="n">
-        <v>268039.4733975241</v>
+        <v>1414759.265074215</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>0: [-5452.431806232475, -6599.60120023246]
-1: [-5235.08859923765, -6144.855215719961]
-2: [-9527.80665745036, -7744.098499917628]</t>
+          <t>0: [-26.697609931773226, 148.26565130386837]
+1: [-434.3645283129735, 442.9621356508567]
+2: [-597.6579675133238, 316.50655698477453]
+3: [-456.10455025675947, 427.09552245385294]
+4: [-7.775064628135619, 34.22217782853513]</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0: -8598.86904677809
-1: -9201.15878678118
-2: 10184.5770415241</t>
+          <t>0: -725.482689486135
+1: 191.564246542724
+2: 873.064106903886
+3: 1146.47175447853
+4: 4275.77622327887</t>
         </is>
       </c>
     </row>
@@ -831,26 +851,30 @@
         <v>30</v>
       </c>
       <c r="F8" t="n">
-        <v>216508.6676031861</v>
+        <v>476422.9439355552</v>
       </c>
       <c r="G8" t="n">
-        <v>69238244762.38664</v>
+        <v>285583958415.5924</v>
       </c>
       <c r="H8" t="n">
-        <v>263131.6111043799</v>
+        <v>534400.5598945349</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>0: [-6424.111312507969, -7794.870992900234]
-1: [-6709.318016813896, -7343.940357510278]
-2: [-11875.763247979901, -9329.855342714398]</t>
+          <t>0: [-38.35186479412417, 148.15400360522418]
+1: [-433.98537507034894, 442.9633356619694]
+2: [-597.0560696472553, 316.50730203152716]
+3: [-458.52255835304976, 427.09242183283726]
+4: [-8.875751315411346, 34.217918642771394]</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>0: -10485.7053271525
-1: -11330.8801489112
-2: 12494.1182908051</t>
+          <t>0: -1040.01001443838
+1: 206.648928397204
+2: 415.080129615783
+3: 1926.24672609747
+4: 6698.55165757296</t>
         </is>
       </c>
     </row>
@@ -873,26 +897,30 @@
         <v>30</v>
       </c>
       <c r="F9" t="n">
-        <v>210222.4200321873</v>
+        <v>477079.6412886294</v>
       </c>
       <c r="G9" t="n">
-        <v>66535848637.65238</v>
+        <v>281180029834.2786</v>
       </c>
       <c r="H9" t="n">
-        <v>257945.4373266803</v>
+        <v>530264.1132815595</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>0: [-7568.345015645405, -8691.821322774875]
-1: [-7671.367453353941, -8438.390174272708]
-2: [-14330.281770000809, -10869.263258573765]</t>
+          <t>0: [-114.07058107014704, 148.10213005137572]
+1: [-429.24071167689203, 442.9672927598399]
+2: [-541.4746865644557, 316.5095482973384]
+3: [-592.1561260809652, 427.08635642013974]
+4: [-10.927779163902551, 34.21329212297717]</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>0: -12406.4372733924
-1: -13493.9175490945
-2: 14730.8661594599</t>
+          <t>0: -2323.77648593119
+1: 352.451348828248
+2: -1275.41970403519
+3: 3183.00088143884
+4: 8922.04290459748</t>
         </is>
       </c>
     </row>
@@ -915,26 +943,30 @@
         <v>30</v>
       </c>
       <c r="F10" t="n">
-        <v>204736.5493581291</v>
+        <v>423996.6812435277</v>
       </c>
       <c r="G10" t="n">
-        <v>64103605663.31059</v>
+        <v>251951026791.9173</v>
       </c>
       <c r="H10" t="n">
-        <v>253186.8986802251</v>
+        <v>501947.2350675092</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>0: [-8987.238491789421, -9714.158646656248]
-1: [-8801.987190159824, -9209.496827434716]
-2: [-16559.51781463371, -12365.703418909987]</t>
+          <t>0: [-126.17483324829067, 148.43209071088557]
+1: [-433.3580597058088, 442.96162852293]
+2: [-372.12622709996094, 316.54918553924665]
+3: [-533.9736236857386, 427.04875640027296]
+4: [-25.608036609467632, 34.18520782400671]</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0: -14298.2557253027
-1: -15723.1792409609
-2: 16753.1194679348</t>
+          <t>0: -2239.25759983508
+1: 261.902188094487
+2: -1439.60946781802
+3: 3225.01857886401
+4: 10354.9979801285</t>
         </is>
       </c>
     </row>
@@ -948,35 +980,39 @@
         <v>9</v>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>3.333</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F11" t="n">
-        <v>199616.5152099403</v>
+        <v>414836.3455997976</v>
       </c>
       <c r="G11" t="n">
-        <v>61850212388.70288</v>
+        <v>264401006418.1617</v>
       </c>
       <c r="H11" t="n">
-        <v>248697.0293121791</v>
+        <v>514199.3839146072</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>0: [-9881.174428002403, -10849.18600601319]
-1: [-10079.020120930849, -10055.020534859217]
-2: [-18624.5179184641, -13821.13483725043]</t>
+          <t>0: [-294.7759568543466, 148.61078010785764]
+1: [-393.51756323406477, 442.961022143693]
+2: [-441.14138725684927, 316.57687282581594]
+3: [-859.2839988433725, 427.08597918386215]
+4: [-112.86758253689354, 34.06579038227216]</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>0: -16046.5793655557
-1: -17841.7306753067
-2: 18690.2892080728</t>
+          <t>0: -2101.05611679085
+1: -179.519538268109
+2: -1764.2520912738
+3: 3919.9509969631
+4: 11199.3418006391</t>
         </is>
       </c>
     </row>
@@ -999,26 +1035,30 @@
         <v>30</v>
       </c>
       <c r="F12" t="n">
-        <v>195441.745648839</v>
+        <v>326622.0900641376</v>
       </c>
       <c r="G12" t="n">
-        <v>59819064513.90353</v>
+        <v>146422917007.9511</v>
       </c>
       <c r="H12" t="n">
-        <v>244579.3624039108</v>
+        <v>382652.475502186</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>0: [-10949.045616912459, -12079.456514968297]
-1: [-11581.623951041365, -10968.870172047054]
-2: [-20554.82105994822, -15238.50596596608]</t>
+          <t>0: [-93.84248194050373, 148.77854844939307]
+1: [-456.6758139240723, 442.9469017090177]
+2: [-527.447706350082, 316.6007736517951]
+3: [-979.3746396223806, 427.0712788676122]
+4: [1.0108896933380978, 34.06593971569962]</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>0: -17667.3769100144
-1: -19964.7174334721
-2: 20312.109296633</t>
+          <t>0: -1729.52735899708
+1: -576.718862170291
+2: -1247.92131178422
+3: 3949.33507722414
+4: 11521.1673076645</t>
         </is>
       </c>
     </row>
@@ -1041,26 +1081,30 @@
         <v>30</v>
       </c>
       <c r="F13" t="n">
-        <v>191374.2148104332</v>
+        <v>439072.1522031694</v>
       </c>
       <c r="G13" t="n">
-        <v>57880244340.34748</v>
+        <v>244715770756.3253</v>
       </c>
       <c r="H13" t="n">
-        <v>240583.1339482206</v>
+        <v>494687.5486166246</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>0: [-12123.431572140777, -13117.59741931116]
-1: [-12490.361667966768, -11944.430946686723]
-2: [-22190.83537649961, -16618.57882534934]</t>
+          <t>0: [41.30175263071138, 148.88165158117778]
+1: [-779.3305452009229, 442.94778786335087]
+2: [-534.8436718987009, 316.61187770690486]
+3: [-906.2913743648237, 427.0719906293399]
+4: [-313.4335354082281, 34.05630241991517]</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>0: -19167.7053507474
-1: -21959.1064215024
-2: 22299.1818476228</t>
+          <t>0: -1653.75828907363
+1: -634.429378869508
+2: -1493.83034142115
+3: 4132.15079539494
+4: 13819.8420677078</t>
         </is>
       </c>
     </row>
@@ -1083,26 +1127,30 @@
         <v>30</v>
       </c>
       <c r="F14" t="n">
-        <v>187618.16536098</v>
+        <v>886144.7404155207</v>
       </c>
       <c r="G14" t="n">
-        <v>56032212423.28486</v>
+        <v>2386987265243.121</v>
       </c>
       <c r="H14" t="n">
-        <v>236711.242705717</v>
+        <v>1544987.788056307</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>0: [-13399.051119159516, -13804.358198974875]
-1: [-13553.202508735265, -12975.508799666854]
-2: [-23799.10866372129, -17962.306539754143]</t>
+          <t>0: [6.0603452855356865, 108.66573525538841]
+1: [-806.3051512148551, 442.9596936939216]
+2: [-457.09181244507533, 316.4951888500551]
+3: [-912.5756604464237, 427.0837960472361]
+4: [-307.73405872260594, 34.39804935562222]</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>0: -21170.3356644311
-1: -23763.7768636095
-2: 24212.5143902002</t>
+          <t>0: -1675.98844631599
+1: -784.758121151597
+2: -1498.96093228524
+3: 3805.96810310839
+4: 14533.7173593995</t>
         </is>
       </c>
     </row>
@@ -1116,35 +1164,39 @@
         <v>13</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>3.333</v>
       </c>
       <c r="E15" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F15" t="n">
-        <v>184119.188115655</v>
+        <v>232014.1623384192</v>
       </c>
       <c r="G15" t="n">
-        <v>54299378268.98658</v>
+        <v>91582421899.03442</v>
       </c>
       <c r="H15" t="n">
-        <v>233022.2698992235</v>
+        <v>302625.8777749094</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>0: [-14848.808698435796, -14520.79769526153]
-1: [-14701.254649857887, -14056.560947030597]
-2: [-25483.75408656728, -19270.938732428167]</t>
+          <t>0: [18.947423028219788, 108.78518383420304]
+1: [-1313.7399478022894, 442.9540873456443]
+2: [-445.82063567184355, 316.53370310548485]
+3: [-907.4812254463919, 427.0809366106331]
+4: [-459.1588973246852, 34.39282983208014]</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0: -23097.3455077181
-1: -25699.706786186
-2: 25958.5483173096</t>
+          <t>0: -1563.85587183487
+1: -2172.31144567729
+2: -2733.51605218604
+3: 4519.92084745692
+4: 16247.9113672454</t>
         </is>
       </c>
     </row>
@@ -1167,26 +1219,30 @@
         <v>30</v>
       </c>
       <c r="F16" t="n">
-        <v>180666.5982408219</v>
+        <v>401508.2261517291</v>
       </c>
       <c r="G16" t="n">
-        <v>52646089370.73504</v>
+        <v>574317356868.2678</v>
       </c>
       <c r="H16" t="n">
-        <v>229447.3564256844</v>
+        <v>757837.2891777415</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>0: [-16028.783111490817, -15266.39694867328]
-1: [-16003.567979692378, -15182.050667699883]
-2: [-27188.26087614302, -20545.19683099365]</t>
+          <t>0: [-92.32621210631301, 91.30905761442074]
+1: [-1324.6275346172254, 442.9593422963978]
+2: [-395.71144954456116, 316.40345411761916]
+3: [-1144.2000547735295, 427.0892748500029]
+4: [-503.344785065408, 34.47191708672191]</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0: -24918.4241228802
-1: -27441.1229218003
-2: 27637.6293203807</t>
+          <t>0: -1458.5832598826
+1: -2154.69214601837
+2: -3088.61972338183
+3: 4634.14563011033
+4: 16422.3644781663</t>
         </is>
       </c>
     </row>
@@ -1209,26 +1265,30 @@
         <v>30</v>
       </c>
       <c r="F17" t="n">
-        <v>177478.4546688547</v>
+        <v>143172.4918651135</v>
       </c>
       <c r="G17" t="n">
-        <v>51086896966.08915</v>
+        <v>29815285778.89105</v>
       </c>
       <c r="H17" t="n">
-        <v>226024.1070463262</v>
+        <v>172671.0334100397</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>0: [-16991.28974475561, -16040.267198840602]
-1: [-17472.543366776386, -16347.07280975956]
-2: [-28974.870355741925, -21786.141380983765]</t>
+          <t>0: [-91.51306609613827, 91.36680468129893]
+1: [-1371.5895799673362, 442.9561469850499]
+2: [-398.6227682586851, 316.4074863094096]
+3: [-1113.8469649590725, 427.0899298324511]
+4: [-496.9154680930314, 34.47157114147153]</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>0: -26617.8004466782
-1: -28998.3318411178
-2: 29049.50853862</t>
+          <t>0: -1420.54561497128
+1: -2267.73303968885
+2: -3019.96323563107
+3: 5273.5790623733
+4: 16495.700278129</t>
         </is>
       </c>
     </row>
@@ -1242,35 +1302,39 @@
         <v>16</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>6.667</v>
       </c>
       <c r="E18" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F18" t="n">
-        <v>174491.0528572915</v>
+        <v>149142.4864629166</v>
       </c>
       <c r="G18" t="n">
-        <v>49559232274.09185</v>
+        <v>33033866574.33166</v>
       </c>
       <c r="H18" t="n">
-        <v>222619.0294518684</v>
+        <v>181752.2120204639</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>0: [-18102.481057346766, -16841.859824455572]
-1: [-18321.70640617973, -17276.901730112626]
-2: [-30845.403617933593, -22993.59482703047]</t>
+          <t>0: [-95.67966273854347, 91.41250499058737]
+1: [-1609.5559192769747, 442.9536453100359]
+2: [-439.4372637377464, 316.4030940039604]
+3: [-1101.8928555152588, 427.0900273789883]
+4: [-406.42989648298504, 34.47173492763318]</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>0: -28378.4562687607
-1: -30428.3859480504
-2: 30823.5242996642</t>
+          <t>0: -1555.35148021498
+1: -2571.21032251944
+2: -2802.0264903308
+3: 5589.97015124434
+4: 15922.1260540015</t>
         </is>
       </c>
     </row>
@@ -1293,26 +1357,30 @@
         <v>30</v>
       </c>
       <c r="F19" t="n">
-        <v>171541.7795688884</v>
+        <v>166383.2555665919</v>
       </c>
       <c r="G19" t="n">
-        <v>47961025449.61362</v>
+        <v>37549614914.1188</v>
       </c>
       <c r="H19" t="n">
-        <v>219000.058104133</v>
+        <v>193777.2301229399</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>0: [-19284.560592268637, -17668.893941916533]
-1: [-19247.18702576925, -17889.151987990677]
-2: [-32797.30860088354, -24165.11958113336]</t>
+          <t>0: [-173.6308968260848, 91.44461455791354]
+1: [-1754.4203021745582, 442.9522281083302]
+2: [-569.6731651314587, 316.3851683954143]
+3: [-864.9444935527084, 427.0909199030838]
+4: [-422.40384347429244, 34.472877833627265]</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>0: -29946.1686933003
-1: -32175.0165455765
-2: 32517.0377956554</t>
+          <t>0: -1500.71575341858
+1: -2672.62656037929
+2: -2877.62730578893
+3: 5802.6575385851
+4: 15431.2014607166</t>
         </is>
       </c>
     </row>
@@ -1326,35 +1394,39 @@
         <v>18</v>
       </c>
       <c r="C20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>3.333</v>
+        <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F20" t="n">
-        <v>168797.3050538367</v>
+        <v>154576.7102820989</v>
       </c>
       <c r="G20" t="n">
-        <v>46501574908.28017</v>
+        <v>37254037614.0489</v>
       </c>
       <c r="H20" t="n">
-        <v>215642.2382286925</v>
+        <v>193013.0503723748</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>0: [-20607.622086699128, -18517.11820270372]
-1: [-20275.742886908985, -18512.52257282244]
-2: [-34591.392483703996, -25302.693102428966]</t>
+          <t>0: [-238.8824071957414, 91.48080134824788]
+1: [-1803.9295833718456, 442.95111968268185]
+2: [-624.8207867343815, 316.36149060368314]
+3: [-448.96843491914575, 427.09212988745713]
+4: [-445.6853462190351, 34.474678108725875]</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>0: -31331.6068065657
-1: -33917.1238383493
-2: 34241.0783623843</t>
+          <t>0: -1378.29977747629
+1: -2486.78873588567
+2: -2556.3601109644
+3: 5773.06910016575
+4: 15409.9278730212</t>
         </is>
       </c>
     </row>
@@ -1377,26 +1449,30 @@
         <v>30</v>
       </c>
       <c r="F21" t="n">
-        <v>166376.9369467609</v>
+        <v>159128.0802303744</v>
       </c>
       <c r="G21" t="n">
-        <v>45116705640.05257</v>
+        <v>40082161138.29169</v>
       </c>
       <c r="H21" t="n">
-        <v>212406.934067729</v>
+        <v>200205.297478093</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>0: [-22085.50459291603, -19384.9162266786]
-1: [-21414.989006452277, -19144.84041962919]
-2: [-36467.607939063, -26407.064410948293]</t>
+          <t>0: [-191.5242063944241, 91.50329614334821]
+1: [-1811.7192767276415, 442.950531718723]
+2: [-769.3137691222753, 316.3308350949995]
+3: [-438.37968779795733, 427.0937348597496]
+4: [-435.7998524230266, 34.47720356439394]</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>0: -32653.658536541
-1: -35530.7374186183
-2: 35682.4213530737</t>
+          <t>0: -1607.71773093071
+1: -2482.13656323812
+2: -2349.9826545453
+3: 5868.15259084676
+4: 15512.8166257398</t>
         </is>
       </c>
     </row>
@@ -1419,26 +1495,30 @@
         <v>30</v>
       </c>
       <c r="F22" t="n">
-        <v>164119.4879026884</v>
+        <v>390517.2094127884</v>
       </c>
       <c r="G22" t="n">
-        <v>43862637362.02408</v>
+        <v>513993541360.1664</v>
       </c>
       <c r="H22" t="n">
-        <v>209434.0883476806</v>
+        <v>716933.4288203936</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>0: [-22931.392773207885, -20271.589557965002]
-1: [-22604.62832805037, -19785.00441736916]
-2: [-38230.403080152944, -27480.495842317014]</t>
+          <t>0: [-17.83213063634983, 81.09551883282356]
+1: [-1662.3586850269014, 442.9547697939666]
+2: [-353.06342337737976, 316.18243579735304]
+3: [-925.5730586205073, 427.104174931563]
+4: [-297.140839646945, 34.58836677717379]</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>0: -34346.6472516706
-1: -37161.1904725052
-2: 36869.7470414146</t>
+          <t>0: -1556.66534621867
+1: -2168.33265355859
+2: -2194.40584876108
+3: 5609.69154954677
+4: 15251.371126794</t>
         </is>
       </c>
     </row>
@@ -1461,26 +1541,30 @@
         <v>30</v>
       </c>
       <c r="F23" t="n">
-        <v>161961.9339334987</v>
+        <v>156378.6701765353</v>
       </c>
       <c r="G23" t="n">
-        <v>42694207073.79636</v>
+        <v>37127472676.19947</v>
       </c>
       <c r="H23" t="n">
-        <v>206625.7657548941</v>
+        <v>192684.905159173</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>0: [-23896.820932234725, -21170.40757366381]
-1: [-23916.358817479006, -20431.629370092895]
-2: [-39477.4296870121, -28524.185976393605]</t>
+          <t>0: [-13.882276809220627, 81.13524820946323]
+1: [-1776.2785084396787, 442.95211247857196]
+2: [-350.8677391323931, 316.1965514493121]
+3: [-932.6030961847733, 427.1025570814621]
+4: [-368.6826693579412, 34.5861353515754]</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>0: -35886.4322723051
-1: -38579.6400164838
-2: 38480.7425878965</t>
+          <t>0: -1553.80398760384
+1: -2411.27090288634
+2: -2194.26228863304
+3: 5615.63629396369
+4: 15627.2019564291</t>
         </is>
       </c>
     </row>
@@ -1494,35 +1578,39 @@
         <v>22</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>3.333</v>
       </c>
       <c r="E24" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F24" t="n">
-        <v>159915.8600260926</v>
+        <v>145517.1408551433</v>
       </c>
       <c r="G24" t="n">
-        <v>41617615917.7994</v>
+        <v>35037256326.2135</v>
       </c>
       <c r="H24" t="n">
-        <v>204003.9605443958</v>
+        <v>187182.4145752306</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>0: [-24953.6061582837, -22071.810929742784]
-1: [-25360.103250475517, -21083.697422723355]
-2: [-40723.296832644664, -29539.82404235318]</t>
+          <t>0: [-81.71716262647186, 81.1536843207989]
+1: [-1627.0483776424285, 442.9508703920795]
+2: [-467.821817043511, 316.1798042120108]
+3: [-828.1674216433807, 427.1032702687066]
+4: [-402.0195146163188, 34.58711529825652]</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>0: -37302.1003952751
-1: -39811.4695250323
-2: 39971.3607300687</t>
+          <t>0: -1507.48751462707
+1: -2256.76596525519
+2: -2455.87629390973
+3: 5801.82271917663
+4: 15442.593629935</t>
         </is>
       </c>
     </row>
@@ -1545,26 +1633,30 @@
         <v>30</v>
       </c>
       <c r="F25" t="n">
-        <v>157932.853331085</v>
+        <v>157479.1029530151</v>
       </c>
       <c r="G25" t="n">
-        <v>40597651834.56184</v>
+        <v>38512439733.00101</v>
       </c>
       <c r="H25" t="n">
-        <v>201488.5898371465</v>
+        <v>196245.8655182346</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>0: [-26047.027965579535, -22976.224834613357]
-1: [-26170.519895065718, -21739.767398853364]
-2: [-42024.36075862223, -30528.01407434173]</t>
+          <t>0: [-217.33788426741697, 81.18458512705148]
+1: [-1590.3290046791972, 442.94935698357307]
+2: [-439.50026525870163, 316.16668995809545]
+3: [-959.7429829614242, 427.1036566352092]
+4: [-433.6327797013255, 34.587715585828995]</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>0: -38702.4386312655
-1: -41399.3210581397
-2: 41397.1461000351</t>
+          <t>0: -1144.27284360182
+1: -2881.9603830129
+2: -2396.77621021303
+3: 6373.52403953444
+4: 16026.3887252801</t>
         </is>
       </c>
     </row>
@@ -1587,26 +1679,30 @@
         <v>30</v>
       </c>
       <c r="F26" t="n">
-        <v>156003.9645212888</v>
+        <v>576832.6979574865</v>
       </c>
       <c r="G26" t="n">
-        <v>39637863423.59154</v>
+        <v>963490086250.9926</v>
       </c>
       <c r="H26" t="n">
-        <v>199092.6001226353</v>
+        <v>981575.3084970061</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>0: [-27245.573592644523, -23884.11246425323]
-1: [-27091.46884158126, -22398.635439510585]
-2: [-43383.23536400152, -31489.73122161146]</t>
+          <t>0: [-63.188554188733995, 67.94828372166991]
+1: [-1630.0172580638805, 442.95800437184886]
+2: [-205.75591515134005, 315.96391315726316]
+3: [-1361.0533927821227, 427.11734999871913]
+4: [-301.100254009921, 34.885539746495624]</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>0: -39911.8299944893
-1: -42921.7414144957
-2: 42589.9896203819</t>
+          <t>0: -675.277616063092
+1: -2977.50272452843
+2: -2648.40540076292
+3: 6901.96556091107
+4: 16544.5306429131</t>
         </is>
       </c>
     </row>
@@ -1620,35 +1716,39 @@
         <v>25</v>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" t="n">
-        <v>0</v>
+        <v>3.333</v>
       </c>
       <c r="E27" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F27" t="n">
-        <v>154149.565149003</v>
+        <v>158004.0899199191</v>
       </c>
       <c r="G27" t="n">
-        <v>38743682149.36143</v>
+        <v>37047582434.67903</v>
       </c>
       <c r="H27" t="n">
-        <v>196834.1488394771</v>
+        <v>192477.4855266949</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>0: [-28559.78991675128, -24796.12698790637]
-1: [-28100.16093962729, -23059.45989800347]
-2: [-44775.19544889652, -32426.323732743676]</t>
+          <t>0: [-59.75606284476873, 67.95819634151718]
+1: [-1747.612214368447, 442.95526034032855]
+2: [-200.80524774212356, 315.98219075464334]
+3: [-1370.9584407117381, 427.1153434707735]
+4: [-370.95393395098256, 34.88298034319257]</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>0: -40957.3978073265
-1: -44327.1560206473
-2: 43965.4810903904</t>
+          <t>0: -673.075145090823
+1: -2939.17080900323
+2: -3014.77346723225
+3: 7393.01343137549
+4: 16995.5178491284</t>
         </is>
       </c>
     </row>
@@ -1671,26 +1771,30 @@
         <v>30</v>
       </c>
       <c r="F28" t="n">
-        <v>152075.6224840587</v>
+        <v>148804.1726333269</v>
       </c>
       <c r="G28" t="n">
-        <v>37762681820.90734</v>
+        <v>32541380264.3784</v>
       </c>
       <c r="H28" t="n">
-        <v>194326.2252525565</v>
+        <v>180392.2954684551</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>0: [-29997.580106537527, -25708.275890391917]
-1: [-29138.56907975429, -23718.304930507788]
-2: [-46223.98048236624, -33334.39519049185]</t>
+          <t>0: [-125.58686085561612, 67.96232356276577]
+1: [-1861.9656889788293, 442.9540904969838]
+2: [-286.306078492092, 315.96671048900305]
+3: [-1277.2340004887715, 427.1162345294896]
+4: [-344.5854276614492, 34.88408478795248]</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>0: -42477.8494020932
-1: -45687.5119640458
-2: 45420.1931797367</t>
+          <t>0: -787.928696202502
+1: -2820.037774677
+2: -3204.36268175594
+3: 6969.5017019227
+4: 16734.2285594969</t>
         </is>
       </c>
     </row>
@@ -1713,26 +1817,30 @@
         <v>30</v>
       </c>
       <c r="F29" t="n">
-        <v>150075.1659558391</v>
+        <v>170993.0535509912</v>
       </c>
       <c r="G29" t="n">
-        <v>36848289082.55358</v>
+        <v>40456604897.65037</v>
       </c>
       <c r="H29" t="n">
-        <v>191959.0817923278</v>
+        <v>201138.2730801136</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>0: [-30796.913571774967, -26620.87125492141]
-1: [-30269.55121839475, -24374.16812639208]
-2: [-47731.98613822698, -34215.02591474336]</t>
+          <t>0: [-481.9345684669056, 67.9827062336225]
+1: [-1910.9591286776263, 442.952865769496]
+2: [-546.0976477152531, 315.9450367899877]
+3: [-1098.4914645899753, 427.1172781524976]
+4: [-457.463181106309, 34.88548020000185]</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>0: -43778.2471967177
-1: -46848.4007007489
-2: 46719.6381020678</t>
+          <t>0: -1687.60109261321
+1: -2583.97107054358
+2: -3368.9518435192
+3: 6631.99904005589
+4: 16382.7913012981</t>
         </is>
       </c>
     </row>
@@ -1746,35 +1854,39 @@
         <v>28</v>
       </c>
       <c r="C30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>3.333</v>
+        <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F30" t="n">
-        <v>148126.7560337639</v>
+        <v>197790.96244884</v>
       </c>
       <c r="G30" t="n">
-        <v>35982032146.94736</v>
+        <v>51139716808.364</v>
       </c>
       <c r="H30" t="n">
-        <v>189689.3042502591</v>
+        <v>226140.9224540397</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>0: [-31710.76982097409, -27533.80502580339]
-1: [-31499.64077072585, -25025.85664978125]
-2: [-49300.511750364356, -35068.673427764064]</t>
+          <t>0: [-427.25619189667674, 68.0453517103158]
+1: [-2152.3929828295195, 442.9509280709392]
+2: [-706.5430849099017, 315.9180587141203]
+3: [-1309.8753136926161, 427.13044248157445]
+4: [-461.0990925975477, 34.88291879800384]</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>0: -44962.1690833651
-1: -47836.0650816689
-2: 47924.1750841818</t>
+          <t>0: -1844.99052695472
+1: -2777.6871356736
+2: -3387.8538075669
+3: 6634.37603740153
+4: 16262.3983632229</t>
         </is>
       </c>
     </row>
@@ -1797,26 +1909,30 @@
         <v>30</v>
       </c>
       <c r="F31" t="n">
-        <v>146537.2171689398</v>
+        <v>173980.023912818</v>
       </c>
       <c r="G31" t="n">
-        <v>35206344228.29495</v>
+        <v>45509583536.22742</v>
       </c>
       <c r="H31" t="n">
-        <v>187633.5370563987</v>
+        <v>213329.7530496565</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>0: [-32710.28483809257, -28446.317882016334]
-1: [-32837.1160678862, -25673.522450754674]
-2: [-50774.65288411642, -35897.582436316276]</t>
+          <t>0: [-227.58181335812313, 68.07571526735907]
+1: [-2171.2698937713953, 442.95051394300026]
+2: [-810.2422540528183, 315.8781460519811]
+3: [-1204.0091817286434, 427.13703331417867]
+4: [-370.98724535591, 34.884639147011974]</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>0: -46084.9816335695
-1: -49292.5432954497
-2: 48916.8509369036</t>
+          <t>0: -1679.55270156471
+1: -2905.59409542265
+2: -3028.45138043368
+3: 6631.81066032393
+4: 16245.9489377128</t>
         </is>
       </c>
     </row>
@@ -1839,26 +1955,30 @@
         <v>30</v>
       </c>
       <c r="F32" t="n">
-        <v>144931.5010313356</v>
+        <v>196660.2325888614</v>
       </c>
       <c r="G32" t="n">
-        <v>34436255293.21225</v>
+        <v>98664179992.22743</v>
       </c>
       <c r="H32" t="n">
-        <v>185570.0818914845</v>
+        <v>314108.5481043574</v>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>0: [-33740.0242655924, -29356.851976126585]
-1: [-34288.71998829949, -26315.41777077208]
-2: [-52312.02055291397, -36701.29431392074]</t>
+          <t>0: [-106.82603564594072, 67.03973218438762]
+1: [-2148.315874880753, 442.95065247771134]
+2: [-742.6463950150688, 315.82113852584473]
+3: [-1356.1479721447517, 427.1431424220834]
+4: [-320.46578731439314, 34.895139278010696]</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>0: -47047.3970728082
-1: -50558.1466890905
-2: 50339.980042482</t>
+          <t>0: -1735.47734468103
+1: -2726.67980494215
+2: -2739.03463690006
+3: 6907.5828102264
+4: 16138.7215490793</t>
         </is>
       </c>
     </row>
@@ -1872,35 +1992,39 @@
         <v>31</v>
       </c>
       <c r="C33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>3.333</v>
+        <v>0</v>
       </c>
       <c r="E33" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F33" t="n">
-        <v>143298.7778761893</v>
+        <v>912594.3754401082</v>
       </c>
       <c r="G33" t="n">
-        <v>33690679043.74653</v>
+        <v>2870181508326.382</v>
       </c>
       <c r="H33" t="n">
-        <v>183550.2085091339</v>
+        <v>1694161.00425148</v>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>0: [-34859.84498078276, -30260.287142635625]
-1: [-35081.022121192356, -26949.96113589495]
-2: [-53212.9867482972, -37479.46893458173]</t>
+          <t>0: [-71.24122707299748, 16.63325443442756]
+1: [-1997.8015417965682, 442.9715720957438]
+2: [-424.6231411488546, 315.15133307633]
+3: [-1733.433468938819, 427.18740814430714]
+4: [-348.8913572936865, 35.423334723345086]</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>0: -47862.4831838321
-1: -51674.0415352849
-2: 51515.4761987948</t>
+          <t>0: -1675.12882887802
+1: -2533.95701441677
+2: -2557.51484284747
+3: 6850.61145860703
+4: 16083.0158208247</t>
         </is>
       </c>
     </row>
@@ -1923,26 +2047,30 @@
         <v>30</v>
       </c>
       <c r="F34" t="n">
-        <v>142193.879280503</v>
+        <v>149552.1645996367</v>
       </c>
       <c r="G34" t="n">
-        <v>33110042809.61987</v>
+        <v>32738263005.48859</v>
       </c>
       <c r="H34" t="n">
-        <v>181961.6520303656</v>
+        <v>180937.1797212739</v>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>0: [-36071.502542882605, -31154.311215268135]
-1: [-35987.035732427496, -27580.256558958274]
-2: [-54139.57922750045, -38237.30415846979]</t>
+          <t>0: [-64.58282886150441, 16.681817106454087]
+1: [-2042.4679913920727, 442.9692238479838]
+2: [-425.23962921073286, 315.15669621602996]
+3: [-1741.592987449261, 427.1932860686653]
+4: [-346.4918635504436, 35.419619842672574]</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>0: -49088.1184397037
-1: -52689.9718507851
-2: 52566.2578584962</t>
+          <t>0: -1673.74168759494
+1: -2577.76884623344
+2: -2569.84864681124
+3: 6905.41259845837
+4: 16128.7618982894</t>
         </is>
       </c>
     </row>
@@ -1965,26 +2093,30 @@
         <v>30</v>
       </c>
       <c r="F35" t="n">
-        <v>141124.9097008426</v>
+        <v>156326.225023671</v>
       </c>
       <c r="G35" t="n">
-        <v>32558228842.05593</v>
+        <v>36247136398.8055</v>
       </c>
       <c r="H35" t="n">
-        <v>180438.9892513698</v>
+        <v>190386.8073129162</v>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>0: [-37379.81135905299, -31773.930643223615]
-1: [-36970.39502037128, -28205.628343260203]
-2: [-55105.05647742743, -38975.11040868357]</t>
+          <t>0: [-72.52378113008915, 16.712459570351427]
+1: [-2102.9655311243287, 442.96789938330244]
+2: [-511.52959681058303, 315.13959557941865]
+3: [-1721.151751101772, 427.2002626922315]
+4: [-318.4438695611289, 35.41856818391323]</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>0: -50139.3805048983
-1: -53551.0728917393
-2: 53508.4521698801</t>
+          <t>0: -1935.73011282287
+1: -3043.76262270302
+2: -2371.75125548614
+3: 7107.05122404068
+4: 16044.4087099567</t>
         </is>
       </c>
     </row>
@@ -1998,35 +2130,39 @@
         <v>34</v>
       </c>
       <c r="C36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>3.333</v>
+        <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F36" t="n">
-        <v>140088.6157241415</v>
+        <v>176855.9514013805</v>
       </c>
       <c r="G36" t="n">
-        <v>32047202905.2129</v>
+        <v>41988281280.21822</v>
       </c>
       <c r="H36" t="n">
-        <v>179017.3257123815</v>
+        <v>204910.4225758617</v>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>0: [-38734.42362515324, -32212.5766697249]
-1: [-37975.86057104944, -28826.03446786783]
-2: [-56111.98080615426, -39694.04246260827]</t>
+          <t>0: [-203.94896274961744, 16.748596989002287]
+1: [-2026.0683403886524, 442.96663613010526]
+2: [-850.006688004861, 315.1170055734433]
+3: [-1698.933550238164, 427.206237953129]
+4: [-401.16406140586406, 35.418965774676046]</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>0: -51094.332811953
-1: -54285.8447825074
-2: 54292.1312312266</t>
+          <t>0: -1733.91965791063
+1: -3312.64544800519
+2: -2240.53991565403
+3: 7301.30591485261
+4: 16205.2148587791</t>
         </is>
       </c>
     </row>
@@ -2040,35 +2176,39 @@
         <v>35</v>
       </c>
       <c r="C37" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>6.667</v>
+        <v>0</v>
       </c>
       <c r="E37" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F37" t="n">
-        <v>139180.205692729</v>
+        <v>195862.7922143118</v>
       </c>
       <c r="G37" t="n">
-        <v>31533881403.77209</v>
+        <v>55145719357.70794</v>
       </c>
       <c r="H37" t="n">
-        <v>177577.8178821107</v>
+        <v>234831.2571990959</v>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>0: [-39469.224315212094, -32646.97832419387]
-1: [-39065.22336369496, -29440.168466948744]
-2: [-57161.076922195025, -40393.762132799704]</t>
+          <t>0: [-288.5337916531998, 16.830820098149196]
+1: [-2315.906727477206, 442.9649428930754]
+2: [-907.6529155379337, 315.08565677463605]
+3: [-1696.8934997058427, 427.2260328161738]
+4: [-403.93062696303815, 35.413446426960725]</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>0: -51935.1148852936
-1: -55417.3266971864
-2: 55484.4820509403</t>
+          <t>0: -1636.49381277159
+1: -3426.15247243178
+2: -2550.83719959899
+3: 7261.66847805821
+4: 16641.2777047458</t>
         </is>
       </c>
     </row>
@@ -2091,26 +2231,30 @@
         <v>30</v>
       </c>
       <c r="F38" t="n">
-        <v>138403.2933278299</v>
+        <v>176606.573808069</v>
       </c>
       <c r="G38" t="n">
-        <v>30995182000.69262</v>
+        <v>47779939872.51944</v>
       </c>
       <c r="H38" t="n">
-        <v>176054.4858863091</v>
+        <v>218586.2298328041</v>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>0: [-40312.88386333706, -33075.8812170943]
-1: [-40242.55922628552, -30045.597901062087]
-2: [-58250.56637886668, -41072.51809935146]</t>
+          <t>0: [-194.69313997918968, 16.86629682184836]
+1: [-2354.971255458142, 442.9644270761118]
+2: [-1052.1047170096451, 315.04393832374126]
+3: [-1518.2991232853453, 427.23406387087095]
+4: [-361.4613681986796, 35.414785793186276]</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>0: -52631.0779265243
-1: -56367.9528598755
-2: 56469.4330836606</t>
+          <t>0: -1511.81571577351
+1: -3302.45732884216
+2: -2801.58545496776
+3: 7146.56582974367
+4: 16328.8604003469</t>
         </is>
       </c>
     </row>
@@ -2124,35 +2268,39 @@
         <v>37</v>
       </c>
       <c r="C39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>3.333</v>
+        <v>0</v>
       </c>
       <c r="E39" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F39" t="n">
-        <v>137689.2839101463</v>
+        <v>168287.7766119037</v>
       </c>
       <c r="G39" t="n">
-        <v>30498920365.94392</v>
+        <v>46066713540.09536</v>
       </c>
       <c r="H39" t="n">
-        <v>174639.4009550649</v>
+        <v>214631.5762885213</v>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>0: [-41227.19043969638, -33499.724864426855]
-1: [-41514.697617217455, -30642.288330177293]
-2: [-59382.38791628011, -41731.24093308816]</t>
+          <t>0: [-178.1624796009485, 16.88220538573965]
+1: [-2342.795155878957, 442.96426350660033]
+2: [-1031.7721511385325, 315.0036591131549]
+3: [-1470.1372254131793, 427.2366792438652]
+4: [-348.4309511350357, 35.41820610064321]</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>0: -53724.4702438553
-1: -57220.7623551992
-2: 57339.193362037</t>
+          <t>0: -1328.15397463889
+1: -3428.34057759918
+2: -3116.40060993265
+3: 6854.6448308929
+4: 15937.184717039</t>
         </is>
       </c>
     </row>
@@ -2175,26 +2323,30 @@
         <v>30</v>
       </c>
       <c r="F40" t="n">
-        <v>137113.6280273887</v>
+        <v>169257.3635346157</v>
       </c>
       <c r="G40" t="n">
-        <v>30033718444.24205</v>
+        <v>46878072170.78522</v>
       </c>
       <c r="H40" t="n">
-        <v>173302.3901861773</v>
+        <v>216513.445704384</v>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>0: [-42218.583010609276, -33918.72965503169]
-1: [-42566.929980110326, -31229.954373482124]
-2: [-60557.818354177354, -42370.579947736835]</t>
+          <t>0: [-179.0122017469467, 16.891451693878707]
+1: [-2297.0464709165667, 442.96432563613746]
+2: [-885.1264644528551, 314.96040661786935]
+3: [-1550.9947970856042, 427.23913740606764]
+4: [-337.90338836450434, 35.42174312958764]</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>0: -54633.9038761897
-1: -57972.8999307164
-2: 58104.7597068569</t>
+          <t>0: -1485.43421830978
+1: -3686.39030286654
+2: -3032.18867028805
+3: 6703.28540267445
+4: 16153.1164680716</t>
         </is>
       </c>
     </row>
@@ -2208,35 +2360,39 @@
         <v>39</v>
       </c>
       <c r="C41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D41" t="n">
-        <v>0</v>
+        <v>3.333</v>
       </c>
       <c r="E41" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F41" t="n">
-        <v>136607.89762631</v>
+        <v>167389.190650366</v>
       </c>
       <c r="G41" t="n">
-        <v>29616365135.04579</v>
+        <v>45518467205.67152</v>
       </c>
       <c r="H41" t="n">
-        <v>172094.0589766125</v>
+        <v>213350.5734833434</v>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>0: [-43230.344441010464, -34333.31935214454]
-1: [-43355.38258644672, -31809.3676772815]
-2: [-61699.18462991793, -42992.23765956309]</t>
+          <t>0: [-182.24183684856112, 16.89938428053413]
+1: [-2258.7950157274404, 442.9643276842967]
+2: [-922.6811140698755, 314.9195129236191]
+3: [-1562.9011466255195, 427.2413621888038]
+4: [-347.0952897603317, 35.42495774167576]</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>0: -55490.5718416587
-1: -58573.4281815988
-2: 58731.5989169184</t>
+          <t>0: -1397.14690379026
+1: -3917.17788026511
+2: -2802.51807061621
+3: 6920.9098377127
+4: 16379.6510655473</t>
         </is>
       </c>
     </row>
@@ -2259,26 +2415,30 @@
         <v>30</v>
       </c>
       <c r="F42" t="n">
-        <v>136113.4865969468</v>
+        <v>168028.050965826</v>
       </c>
       <c r="G42" t="n">
-        <v>29198486778.68197</v>
+        <v>45320183332.15585</v>
       </c>
       <c r="H42" t="n">
-        <v>170875.6471200094</v>
+        <v>212885.376041089</v>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>0: [-44327.13621644495, -34742.90999365721]
-1: [-44206.41851649719, -32379.217526017317]
-2: [-62889.06837939991, -43595.69245969595]</t>
+          <t>0: [-177.00273697554888, 16.90654718776231]
+1: [-2221.375772201521, 442.964368155373]
+2: [-891.1598361360308, 314.8792429838497]
+3: [-1335.538533632766, 427.24352643618175]
+4: [-346.7693800773472, 35.428219959594244]</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>0: -56215.3074650283
-1: -59549.1063023723
-2: 59721.0298459177</t>
+          <t>0: -1297.51097104792
+1: -3647.25368379996
+2: -2573.25317401843
+3: 6903.14386035807
+4: 16378.2485141287</t>
         </is>
       </c>
     </row>
@@ -2292,35 +2452,39 @@
         <v>41</v>
       </c>
       <c r="C43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D43" t="n">
-        <v>0</v>
+        <v>3.333</v>
       </c>
       <c r="E43" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F43" t="n">
-        <v>135586.951937725</v>
+        <v>169387.4363910132</v>
       </c>
       <c r="G43" t="n">
-        <v>28795305096.60624</v>
+        <v>46553357672.73396</v>
       </c>
       <c r="H43" t="n">
-        <v>169691.7944292129</v>
+        <v>215762.2711984974</v>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>0: [-45512.00872317998, -35145.81465388142]
-1: [-45124.07048278357, -32938.64413385326]
-2: [-63509.93826115587, -44180.688614106715]</t>
+          <t>0: [-145.0277698272448, 16.914253336954808]
+1: [-2118.794501790954, 442.9646515286295]
+2: [-667.0489780728627, 314.8356770651437]
+3: [-1279.8278294404324, 427.24590244160737]
+4: [-330.0850827283424, 35.4316228799729]</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>0: -56815.4768209088
-1: -60335.8463387664
-2: 60489.3350967512</t>
+          <t>0: -1399.77642850047
+1: -3287.41678658569
+2: -2779.8944930574
+3: 7073.85221965686
+4: 16551.5767649249</t>
         </is>
       </c>
     </row>
@@ -2343,26 +2507,30 @@
         <v>30</v>
       </c>
       <c r="F44" t="n">
-        <v>135212.0085395194</v>
+        <v>168232.1103649194</v>
       </c>
       <c r="G44" t="n">
-        <v>28487860321.23613</v>
+        <v>40892908239.47263</v>
       </c>
       <c r="H44" t="n">
-        <v>168783.4717063141</v>
+        <v>202219.9501519883</v>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>0: [-46788.88472623736, -35542.357123635404]
-1: [-46057.388928897424, -33490.94944638933]
-2: [-64180.32722426167, -44751.20950652121]</t>
+          <t>0: [-176.51088523253847, 16.938863022594433]
+1: [-2164.4576657641715, 442.96384507993497]
+2: [-679.8322782623202, 314.8108249806831]
+3: [-1235.0405077431942, 427.2474507418735]
+4: [-342.666675464826, 35.43401008264716]</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>0: -57315.0262328654
-1: -61042.4296932641
-2: 61160.6107449802</t>
+          <t>0: -2081.96694504967
+1: -3001.61158683716
+2: -3206.77281667009
+3: 7384.76776335035
+4: 16499.766381084</t>
         </is>
       </c>
     </row>
@@ -2385,26 +2553,30 @@
         <v>30</v>
       </c>
       <c r="F45" t="n">
-        <v>134844.1383430091</v>
+        <v>207121.831088676</v>
       </c>
       <c r="G45" t="n">
-        <v>28198860296.92548</v>
+        <v>87793509479.10867</v>
       </c>
       <c r="H45" t="n">
-        <v>167925.1627866577</v>
+        <v>296299.6953746471</v>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>0: [-47468.112225845354, -35932.968172221175]
-1: [-47066.11637212066, -34036.106735310575]
-2: [-64877.72369828717, -45307.78772939834]</t>
+          <t>0: [-73.12975363944273, 14.235419522855869]
+1: [-2172.5790180336285, 442.96399088767953]
+2: [-703.8132419261137, 314.7547404503614]
+3: [-1398.249468123256, 427.2630014856083]
+4: [-319.2700070188449, 35.441283411834924]</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>0: -58123.2712159261
-1: -61651.5845967409
-2: 61724.0803802667</t>
+          <t>0: -2526.08368095286
+1: -2657.13165791632
+2: -3236.59548211738
+3: 7154.9368926848
+4: 16412.0068485581</t>
         </is>
       </c>
     </row>
@@ -2427,26 +2599,30 @@
         <v>30</v>
       </c>
       <c r="F46" t="n">
-        <v>134486.2562272737</v>
+        <v>189986.3048310708</v>
       </c>
       <c r="G46" t="n">
-        <v>27933047680.51582</v>
+        <v>58363521422.59228</v>
       </c>
       <c r="H46" t="n">
-        <v>167131.827251771</v>
+        <v>241585.4329685304</v>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>0: [-48258.71137055842, -36318.264629140365]
-1: [-48156.51387695723, -34574.53684352039]
-2: [-65604.17946852441, -45851.36914922088]</t>
+          <t>0: [-238.9303958313914, 14.285458008522653]
+1: [-2404.416694960043, 442.96314885161763]
+2: [-407.12818792127763, 314.7177964082508]
+3: [-1204.2471414597428, 427.2842423631978]
+4: [-293.91486864631804, 35.43237976069705]</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>0: -58848.6631442122
-1: -62159.6740515788
-2: 62187.9254937853</t>
+          <t>0: -2502.13486782878
+1: -2605.74011169681
+2: -3017.92328965648
+3: 7206.72665849952
+4: 16666.7889652259</t>
         </is>
       </c>
     </row>
@@ -2469,26 +2645,30 @@
         <v>30</v>
       </c>
       <c r="F47" t="n">
-        <v>134115.0610149916</v>
+        <v>197327.2820057744</v>
       </c>
       <c r="G47" t="n">
-        <v>27663056755.50027</v>
+        <v>63501743512.16398</v>
       </c>
       <c r="H47" t="n">
-        <v>166322.1475195059</v>
+        <v>251995.5228018228</v>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>0: [-49112.42851267725, -36698.05710207816]
-1: [-49334.219778373226, -35105.37392681364]
-2: [-66384.82782789238, -46381.719202440465]</t>
+          <t>0: [-519.7868540702902, 14.33760084947632]
+1: [-2272.8072898738474, 442.9618987070665]
+2: [-517.4513084885967, 314.68441303439533]
+3: [-1144.7806686503416, 427.3102251948866]
+4: [-407.2329956667963, 35.4173461056687]</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>0: -59414.2575804285
-1: -62581.5316359495
-2: 63002.6092528725</t>
+          <t>0: -2644.98064849762
+1: -2550.3599410382
+2: -2869.21612036589
+3: 6999.04799385933
+4: 16603.1706180271</t>
         </is>
       </c>
     </row>
@@ -2511,26 +2691,30 @@
         <v>30</v>
       </c>
       <c r="F48" t="n">
-        <v>133695.1261161909</v>
+        <v>190177.9122597663</v>
       </c>
       <c r="G48" t="n">
-        <v>27372049495.37545</v>
+        <v>55340019891.03044</v>
       </c>
       <c r="H48" t="n">
-        <v>165445.0044436986</v>
+        <v>235244.5958806077</v>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>0: [-50033.309640277235, -37071.13739829462]
-1: [-50603.49360571126, -35626.52371048715]
-2: [-67194.3473883929, -46897.15786692632]</t>
+          <t>0: [-639.7261573512769, 14.375987523554477]
+1: [-2495.1131311629792, 442.96113308394024]
+2: [-439.731535380003, 314.64219372258964]
+3: [-796.8152229429492, 427.32760385218205]
+4: [-370.37088446305916, 35.41188097811063]</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>0: -59877.383334196
-1: -63328.3022555899
-2: 63627.3364889299</t>
+          <t>0: -2840.05066894558
+1: -2441.8260807065
+2: -2669.09655611864
+3: 6634.69250362733
+4: 16161.2702358059</t>
         </is>
       </c>
     </row>
@@ -2553,26 +2737,30 @@
         <v>30</v>
       </c>
       <c r="F49" t="n">
-        <v>133318.8643585456</v>
+        <v>169696.764538765</v>
       </c>
       <c r="G49" t="n">
-        <v>27103904400.21795</v>
+        <v>47129921815.61763</v>
       </c>
       <c r="H49" t="n">
-        <v>164632.6346755647</v>
+        <v>217094.2694214143</v>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>0: [-50967.333835687314, -37437.88739742007]
-1: [-51273.648452702735, -36138.161320828964]
-2: [-68033.88315722476, -47398.27289297033]</t>
+          <t>0: [-474.87158329145433, 14.388576867509471]
+1: [-2434.832991842961, 442.9611818100885]
+2: [-362.80872469316415, 314.59788191626666]
+3: [-733.0792238214749, 427.3301855065005]
+4: [-321.13230322116533, 35.41461216611119]</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>0: -60263.0136020531
-1: -63963.0379764331
-2: 64167.1072341071</t>
+          <t>0: -2778.67096843709
+1: -2219.70062979054
+2: -2921.72222235289
+3: 6549.08734209957
+4: 16293.8833858582</t>
         </is>
       </c>
     </row>
@@ -2595,26 +2783,30 @@
         <v>30</v>
       </c>
       <c r="F50" t="n">
-        <v>132957.7725014048</v>
+        <v>180295.4626351061</v>
       </c>
       <c r="G50" t="n">
-        <v>26855247118.0368</v>
+        <v>49646401946.85658</v>
       </c>
       <c r="H50" t="n">
-        <v>163875.7063082774</v>
+        <v>222814.725605954</v>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>0: [-51976.08772375861, -37798.637235363196]
-1: [-52058.072880023225, -36640.42031243102]
-2: [-68904.5087458583, -47885.669099253246]</t>
+          <t>0: [-597.6172827817616, 14.40403560736299]
+1: [-2463.157579194733, 442.9611203392609]
+2: [-375.5685029037084, 314.5538463981911]
+3: [-658.7740790717423, 427.33807509110864]
+4: [-338.84427706909116, 35.41487495792571]</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>0: -60979.5368463269
-1: -64413.676123436
-2: 64595.6406222653</t>
+          <t>0: -2732.37574712554
+1: -2279.95145653338
+2: -2878.72037624014
+3: 6518.2983633668
+4: 16077.7432604393</t>
         </is>
       </c>
     </row>
@@ -2628,35 +2820,39 @@
         <v>49</v>
       </c>
       <c r="C51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D51" t="n">
-        <v>0</v>
+        <v>3.333</v>
       </c>
       <c r="E51" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F51" t="n">
-        <v>132600.609800584</v>
+        <v>176817.4395859108</v>
       </c>
       <c r="G51" t="n">
-        <v>26630329741.85298</v>
+        <v>47647643455.033</v>
       </c>
       <c r="H51" t="n">
-        <v>163188.0196027055</v>
+        <v>218283.401693837</v>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>0: [-53066.42844061133, -38154.21051413305]
-1: [-52904.1912036286, -37134.33913446044]
-2: [-69791.52683027333, -48360.719091236344]</t>
+          <t>0: [-649.6947063454946, 14.420996709956688]
+1: [-2491.515119115189, 442.96104764082213]
+2: [-380.29546461232485, 314.5115070813273]
+3: [-893.445724487499, 427.3452543958436]
+4: [-332.8058187591016, 35.41520749357468]</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>0: -61519.587628685
-1: -64780.7874107592
-2: 64942.1515764659</t>
+          <t>0: -2697.14809168449
+1: -2327.36368407362
+2: -2549.80226601581
+3: 6612.36333547676
+4: 15958.5237869888</t>
         </is>
       </c>
     </row>
@@ -2679,26 +2875,30 @@
         <v>30</v>
       </c>
       <c r="F52" t="n">
-        <v>132247.3712335763</v>
+        <v>194334.5393038372</v>
       </c>
       <c r="G52" t="n">
-        <v>26402882990.06155</v>
+        <v>57099427383.99997</v>
       </c>
       <c r="H52" t="n">
-        <v>162489.6396391522</v>
+        <v>238954.8647422772</v>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>0: [-54244.87057325424, -38504.024292841095]
-1: [-53815.979281351465, -37618.73083470609]
-2: [-70716.59736442554, -48822.82646760071]</t>
+          <t>0: [-625.9273651053952, 14.452671590968492]
+1: [-2510.940528289852, 442.9607011971003]
+2: [-397.4649915899746, 314.4676167654912]
+3: [-914.599215228387, 427.3637004695627]
+4: [-335.5939229387373, 35.40902390636539]</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>0: -61986.545544188
-1: -65076.7632479558
-2: 65603.6646129918</t>
+          <t>0: -2744.44540308888
+1: -2178.28647394962
+2: -2361.11220370973
+3: 6711.300207585
+4: 16231.9558929086</t>
         </is>
       </c>
     </row>
@@ -2712,35 +2912,39 @@
         <v>51</v>
       </c>
       <c r="C53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D53" t="n">
-        <v>3.333</v>
+        <v>0</v>
       </c>
       <c r="E53" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F53" t="n">
-        <v>131859.5511125033</v>
+        <v>177010.1482323357</v>
       </c>
       <c r="G53" t="n">
-        <v>26176563572.16142</v>
+        <v>47450476092.56109</v>
       </c>
       <c r="H53" t="n">
-        <v>161791.7289979974</v>
+        <v>217831.3019117342</v>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>0: [-54862.25468586644, -38846.70194630699]
-1: [-54737.81453228683, -38092.82562066578]
-2: [-71117.34010789667, -49271.48006053936]</t>
+          <t>0: [-699.1914562985021, 14.465420295733566]
+1: [-2424.615524599423, 442.96085818772303]
+2: [-338.20612054207123, 314.4161503812009]
+3: [-374.2995624457815, 427.36933013973703]
+4: [-373.4011215868416, 35.41137410458605]</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>0: -62316.8008391482
-1: -65686.2414661114
-2: 66151.5674049329</t>
+          <t>0: -2879.65293200103
+1: -1880.33754996968
+2: -2157.09305207201
+3: 6850.78771533487
+4: 16238.4021907082</t>
         </is>
       </c>
     </row>
@@ -2763,26 +2967,30 @@
         <v>29</v>
       </c>
       <c r="F54" t="n">
-        <v>131610.5494120446</v>
+        <v>159999.3886409165</v>
       </c>
       <c r="G54" t="n">
-        <v>26013349196.3171</v>
+        <v>41739191882.95413</v>
       </c>
       <c r="H54" t="n">
-        <v>161286.5437546391</v>
+        <v>204301.7177679966</v>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>0: [-55589.77352797213, -39183.054345953]
-1: [-55732.5991832111, -38559.54834477298]
-2: [-71587.9620606043, -49709.61296224282]</t>
+          <t>0: [-692.709872608497, 14.483056217194827]
+1: [-2418.0884297690427, 442.96034319433727]
+2: [-284.2582256757208, 314.3828452469861]
+3: [-254.98543825059897, 427.3713199269357]
+4: [-352.99508258958343, 35.41350689537161]</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>0: -62577.1086791967
-1: -66124.9137180136
-2: 66492.0789622397</t>
+          <t>0: -3257.55156213125
+1: -1986.15962881082
+2: -2174.92730265649
+3: 6513.44558159184
+4: 16104.8044406724</t>
         </is>
       </c>
     </row>
@@ -2805,26 +3013,30 @@
         <v>29</v>
       </c>
       <c r="F55" t="n">
-        <v>131439.6938781848</v>
+        <v>163018.6131770309</v>
       </c>
       <c r="G55" t="n">
-        <v>25868912761.10106</v>
+        <v>43152410052.90393</v>
       </c>
       <c r="H55" t="n">
-        <v>160838.1570433492</v>
+        <v>207731.5817416888</v>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>0: [-56374.14860659838, -39514.37538548722]
-1: [-56807.16282431522, -39020.27936957972]
-2: [-72077.79673478805, -50138.81295406944]</t>
+          <t>0: [-625.4938159424097, 14.49807434011123]
+1: [-2392.7531455832873, 442.9600386418193]
+2: [-249.6866936519388, 314.34711402717306]
+3: [-107.5844582736998, 427.3734482446559]
+4: [-337.9760793143386, 35.41602701193405]</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>0: -63159.333930951
-1: -66503.5878219385
-2: 66766.180666818</t>
+          <t>0: -3272.02464039676
+1: -2048.22627755517
+2: -1972.59599999115
+3: 6395.17753390824
+4: 16086.4991020892</t>
         </is>
       </c>
     </row>
@@ -2847,26 +3059,30 @@
         <v>30</v>
       </c>
       <c r="F56" t="n">
-        <v>131282.0624229326</v>
+        <v>164864.4424523819</v>
       </c>
       <c r="G56" t="n">
-        <v>25733253964.21145</v>
+        <v>43926371440.6628</v>
       </c>
       <c r="H56" t="n">
-        <v>160415.8781549116</v>
+        <v>209586.1909589055</v>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>0: [-57220.253937050176, -39840.95090765505]
-1: [-57967.95417598754, -39475.1779791936]
-2: [-72587.70338013522, -50559.442649423676]</t>
+          <t>0: [-443.51732268600466, 14.509905906360471]
+1: [-2329.443387666928, 442.95996106105554]
+2: [-229.48527517749864, 314.30790679860314]
+3: [-5.049892851263444, 427.3757920131456]
+4: [-320.5776323223771, 35.41921282642958]</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>0: -63567.0957812335
-1: -66775.6090931192
-2: 66986.1270918774</t>
+          <t>0: -3471.30236965246
+1: -2297.55273508261
+2: -1980.25445696989
+3: 6591.92830783492
+4: 16300.7187202651</t>
         </is>
       </c>
     </row>
@@ -2880,35 +3096,39 @@
         <v>55</v>
       </c>
       <c r="C57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D57" t="n">
-        <v>3.333</v>
+        <v>0</v>
       </c>
       <c r="E57" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F57" t="n">
-        <v>131106.079488506</v>
+        <v>164344.8726736569</v>
       </c>
       <c r="G57" t="n">
-        <v>25592566777.86665</v>
+        <v>44462481159.08195</v>
       </c>
       <c r="H57" t="n">
-        <v>159976.7694944071</v>
+        <v>210861.2841635039</v>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>0: [-58076.736281473866, -40162.68758425599]
-1: [-58574.09328422316, -39923.60737000633]
-2: [-73163.48088870927, -50971.337053055126]</t>
+          <t>0: [-117.53761747696004, 14.519046743873464]
+1: [-2224.112421995707, 442.95989098289914]
+2: [-590.0739447509769, 314.2671021809615]
+3: [219.01142121753674, 427.3781629944532]
+4: [-325.8950707486037, 35.42260120909635]</t>
         </is>
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>0: -63992.2630983438
-1: -66980.4183023588
-2: 67517.6003701815</t>
+          <t>0: -3137.29753667401
+1: -2528.36013813249
+2: -1938.06356840037
+3: 6759.5944755754
+4: 16503.227103042</t>
         </is>
       </c>
     </row>
@@ -2922,35 +3142,39 @@
         <v>56</v>
       </c>
       <c r="C58" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D58" t="n">
-        <v>3.333</v>
+        <v>0</v>
       </c>
       <c r="E58" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F58" t="n">
-        <v>130961.1190675496</v>
+        <v>168172.2415935725</v>
       </c>
       <c r="G58" t="n">
-        <v>25434289578.4934</v>
+        <v>45970416248.15781</v>
       </c>
       <c r="H58" t="n">
-        <v>159481.3141985399</v>
+        <v>214407.1273259306</v>
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>0: [-58999.47869335907, -40478.34204292788]
-1: [-59293.51612257796, -40363.60848770788]
-2: [-73759.92798037261, -51372.83062190482]</t>
+          <t>0: [-118.89155241761088, 14.534908755512891]
+1: [-2129.217651717879, 442.9598249318722]
+2: [-715.7526218921597, 314.22803977325]
+3: [78.09627960076983, 427.3803310476942]
+4: [-340.4728025427811, 35.425761491321076]</t>
         </is>
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>0: -64226.1670058589
-1: -67478.6701187947
-2: 67870.6320240556</t>
+          <t>0: -2691.51536709352
+1: -2251.48981082051
+2: -1945.40295420392
+3: 6986.77578135769
+4: 16520.5072095359</t>
         </is>
       </c>
     </row>
@@ -2973,26 +3197,30 @@
         <v>30</v>
       </c>
       <c r="F59" t="n">
-        <v>130880.7421537226</v>
+        <v>1133055.855840238</v>
       </c>
       <c r="G59" t="n">
-        <v>25288679652.04699</v>
+        <v>4879602696295.439</v>
       </c>
       <c r="H59" t="n">
-        <v>159024.1480154728</v>
+        <v>2208982.276138819</v>
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>0: [-59994.15426857682, -40788.18402675153]
-1: [-60068.85849773231, -40795.35323275128]
-2: [-74377.59799862311, -51764.24420489977]</t>
+          <t>0: [6.0834002590419125, -49.72428265986572]
+1: [-1965.056519490488, 442.9836281880006]
+2: [-374.30754935275576, 313.41465758244215]
+3: [-292.92539683314936, 427.43593327459223]
+4: [-324.6990788794672, 35.64043385081866]</t>
         </is>
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>0: -64407.0582579566
-1: -67802.8426328302
-2: 68161.7119782296</t>
+          <t>0: -2396.87384859243
+1: -2032.13254596049
+2: -2065.2195574165
+3: 6889.85841443048
+4: 16400.3261567323</t>
         </is>
       </c>
     </row>
@@ -3015,26 +3243,30 @@
         <v>30</v>
       </c>
       <c r="F60" t="n">
-        <v>130807.3735772433</v>
+        <v>145258.5628142972</v>
       </c>
       <c r="G60" t="n">
-        <v>25156043812.25216</v>
+        <v>32686927770.38257</v>
       </c>
       <c r="H60" t="n">
-        <v>158606.5692594483</v>
+        <v>180795.2647897134</v>
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>0: [-61067.16128341842, -41092.60013052101]
-1: [-60904.5804761529, -41219.192570081934]
-2: [-75017.5192974623, -52146.149270718124]</t>
+          <t>0: [8.328456134191049, -49.67129365199028]
+1: [-2057.269384494466, 442.9810171625745]
+2: [-368.365345932857, 313.4346478034546]
+3: [-298.00825524588765, 427.43377808064304]
+4: [-353.1622924501635, 35.637479743403695]</t>
         </is>
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>0: -64545.4941660849
-1: -68145.3221262438
-2: 68335.1106918528</t>
+          <t>0: -2389.42581396417
+1: -2213.12130503494
+2: -2179.27492002053
+3: 6996.31261223463
+4: 16517.325914349</t>
         </is>
       </c>
     </row>
@@ -3048,35 +3280,39 @@
         <v>59</v>
       </c>
       <c r="C61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D61" t="n">
-        <v>0</v>
+        <v>3.333</v>
       </c>
       <c r="E61" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F61" t="n">
-        <v>130704.7926950758</v>
+        <v>141516.9416171767</v>
       </c>
       <c r="G61" t="n">
-        <v>25033061555.02317</v>
+        <v>30234054872.86532</v>
       </c>
       <c r="H61" t="n">
-        <v>158218.3982823211</v>
+        <v>173879.4262495288</v>
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>0: [-62226.0757735465, -41392.58132417647]
-1: [-61750.27868056772, -41636.23568008921]
-2: [-75716.06118605126, -52519.66606218833]</t>
+          <t>0: [5.53405522371198, -49.636038907217674]
+1: [-2184.804736042695, 442.9792430969131]
+2: [-363.26110632163324, 313.43272592085543]
+3: [-304.8032791496743, 427.4337339531529]
+4: [-305.5238276970551, 35.637501421573035]</t>
         </is>
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>0: -64961.7408672847
-1: -68300.4025983471
-2: 68469.8388003884</t>
+          <t>0: -2470.29309595621
+1: -2227.24519684044
+2: -2464.75320209581
+3: 7031.61038910141
+4: 16552.5276462882</t>
         </is>
       </c>
     </row>
@@ -3099,26 +3335,30 @@
         <v>30</v>
       </c>
       <c r="F62" t="n">
-        <v>130644.0080063198</v>
+        <v>172800.2078025552</v>
       </c>
       <c r="G62" t="n">
-        <v>24925410257.6758</v>
+        <v>40732242544.52671</v>
       </c>
       <c r="H62" t="n">
-        <v>157877.8333322186</v>
+        <v>201822.3043781998</v>
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>0: [-62825.99236119128, -41687.627667111585]
-1: [-62662.56514376568, -42046.54693886037]
-2: [-75951.33793102333, -52885.13783825181]</t>
+          <t>0: [-88.57466797588707, -49.61468447892872]
+1: [-2014.5436402725136, 442.9782163389168]
+2: [-521.1480589452066, 313.4088432918502]
+3: [-237.82877964826446, 427.4350396027631]
+4: [-361.2524513339606, 35.63940087670551]</t>
         </is>
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>0: -65284.7602059549
-1: -68417.555213699
-2: 68868.9900655534</t>
+          <t>0: -2347.88824080568
+1: -2044.49634872833
+2: -2420.0066157523
+3: 6914.09141911357
+4: 16803.3030552414</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
♻️ Refactor: Harden atomic_train_a_model with pre-run DB cleanup for LR sweep integrity
✅ Moved WeightAdjustments table cleanup into atomic_train_a_model to guarantee fresh state before every sweep run.
✅ Prevents contamination of training results from earlier runs and ensures sweep logic uses clean model state.
✅ Simplifies control flow by removing implicit cleanup and tying it directly to sweep detection.
✅ Verified: deterministic sweep results, consistent model behavior, no more constraint violations.

🧠 Insight: Sweep logic is now atomic in both config and DB — no stale values, no misleading winners.

Next: Add target scaler + dynamic thresholding for NF visualization.
</commit_message>
<xml_diff>
--- a/src/reports/_XL_Template.xlsx
+++ b/src/reports/_XL_Template.xlsx
@@ -536,10 +536,10 @@
     <col width="10" customWidth="1" min="4" max="4"/>
     <col width="7" customWidth="1" min="5" max="5"/>
     <col width="21" customWidth="1" min="6" max="6"/>
-    <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="21" customWidth="1" min="7" max="7"/>
     <col width="25" customWidth="1" min="8" max="8"/>
-    <col width="69" customWidth="1" min="9" max="9"/>
-    <col width="41" customWidth="1" min="10" max="10"/>
+    <col width="27" customWidth="1" min="9" max="9"/>
+    <col width="24" customWidth="1" min="10" max="10"/>
     <col width="25" customWidth="1" style="4" min="11" max="16384"/>
   </cols>
   <sheetData>
@@ -605,2760 +605,2622 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>33.333</v>
       </c>
       <c r="E3" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F3" t="n">
-        <v>15626.5454045192</v>
+        <v>0.855037503005838</v>
       </c>
       <c r="G3" t="n">
-        <v>300854828.3290483</v>
+        <v>1.061973967007349</v>
       </c>
       <c r="H3" t="n">
-        <v>17345.16729031601</v>
+        <v>1.030521211333056</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>0: [36.05897508073254, 326.57783390390426]
-1: [4.492312441329078]</t>
+          <t>0: [-1.7121526374948117]</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>0: 1.81757328780406
-1: 2.73242475583795</t>
+          <t>0: 1.00445880336338</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>2</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>36.667</v>
       </c>
       <c r="E4" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F4" t="n">
-        <v>15620.36443826622</v>
+        <v>0.7766832023499021</v>
       </c>
       <c r="G4" t="n">
-        <v>300657574.7714426</v>
+        <v>0.8010968240864905</v>
       </c>
       <c r="H4" t="n">
-        <v>17339.48023360108</v>
+        <v>0.8950401242885654</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>0: [110.08192939212267, 1001.3806893006175]
-1: [7.492312441329078]</t>
+          <t>0: [-1.4099377998623837]</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>0: 8.73746419226118
-1: 5.73242475583795</t>
+          <t>0: 0.972280829424464</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>36.667</v>
       </c>
       <c r="E5" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F5" t="n">
-        <v>15614.36443826622</v>
+        <v>0.7272647999708628</v>
       </c>
       <c r="G5" t="n">
-        <v>300470166.3981834</v>
+        <v>0.657705989990908</v>
       </c>
       <c r="H5" t="n">
-        <v>17334.07529688802</v>
+        <v>0.8109907459341987</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>0: [223.47395409815437, 2038.256265914903]
-1: [10.492312441329078]</t>
+          <t>0: [-1.1453153257774356]</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>0: 19.4371241712445
-1: 8.73242475583795</t>
+          <t>0: 0.892416063241772</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>36.667</v>
       </c>
       <c r="E6" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F6" t="n">
-        <v>15608.36443826622</v>
+        <v>0.6881221959920591</v>
       </c>
       <c r="G6" t="n">
-        <v>300282830.0249242</v>
+        <v>0.5579971943655522</v>
       </c>
       <c r="H6" t="n">
-        <v>17328.67075181834</v>
+        <v>0.7469920979271147</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>0: [376.2350491988276, 3437.2045637467604]
-1: [13.492312441329078]</t>
+          <t>0: [-0.9039711145958529]</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>0: 33.9165532247541
-1: 11.732424755838</t>
+          <t>0: 0.795479529278569</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E7" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F7" t="n">
-        <v>15602.36443826622</v>
+        <v>0.6543258129245486</v>
       </c>
       <c r="G7" t="n">
-        <v>300095565.651665</v>
+        <v>0.4818262616421801</v>
       </c>
       <c r="H7" t="n">
-        <v>17323.26659875859</v>
+        <v>0.6941370625763907</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>0: [568.3652146941424, 5198.22558279619]
-1: [16.492312441329076]</t>
+          <t>0: [-0.6793116619165521]</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0: 52.1757513527899
-1: 14.732424755838</t>
+          <t>0: 0.694843892287312</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>56.667</v>
       </c>
       <c r="E8" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F8" t="n">
-        <v>15596.36443826622</v>
+        <v>0.6236685481245602</v>
       </c>
       <c r="G8" t="n">
-        <v>299908373.2784058</v>
+        <v>0.421903080756927</v>
       </c>
       <c r="H8" t="n">
-        <v>17317.86283807577</v>
+        <v>0.6495406690553925</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>0: [799.8644505840987, 7321.319323063192]
-1: [19.492312441329076]</t>
+          <t>0: [-0.4682002236042681]</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>0: 74.214718555352
-1: 17.732424755838</t>
+          <t>0: 0.596187820155388</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>7</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>56.667</v>
       </c>
       <c r="E9" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F9" t="n">
-        <v>15590.36443826622</v>
+        <v>0.595159187313048</v>
       </c>
       <c r="G9" t="n">
-        <v>299721252.9051467</v>
+        <v>0.3746163955989005</v>
       </c>
       <c r="H9" t="n">
-        <v>17312.4594701373</v>
+        <v>0.6120591438732866</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>0: [1070.7327568686965, 9806.485784547767]
-1: [22.492312441329076]</t>
+          <t>0: [-0.2690039081571134]</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>0: 100.03345483244
-1: 20.732424755838</t>
+          <t>0: 0.501783899906535</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>8</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>56.667</v>
       </c>
       <c r="E10" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F10" t="n">
-        <v>15584.36443826622</v>
+        <v>0.5683388779473336</v>
       </c>
       <c r="G10" t="n">
-        <v>299534204.5318875</v>
+        <v>0.3376973286806814</v>
       </c>
       <c r="H10" t="n">
-        <v>17307.05649531102</v>
+        <v>0.5811173106014665</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>0: [1380.9701335479358, 12653.724967249913]
-1: [25.492312441329076]</t>
+          <t>0: [-0.08072957527603863]</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0: 129.631960184055
-1: 23.732424755838</t>
+          <t>0: 0.412412166362175</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>9</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>56.667</v>
       </c>
       <c r="E11" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F11" t="n">
-        <v>15578.36443826622</v>
+        <v>0.5429778889137717</v>
       </c>
       <c r="G11" t="n">
-        <v>299347228.1586282</v>
+        <v>0.3094932357771391</v>
       </c>
       <c r="H11" t="n">
-        <v>17301.65391396523</v>
+        <v>0.5563211624386933</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>0: [1730.5765806218167, 15863.036871169632]
-1: [28.492312441329076]</t>
+          <t>0: [0.0973477003802295]</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>0: 163.010234610196
-1: 26.732424755838</t>
+          <t>0: 0.328207386788371</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>10</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>56.667</v>
       </c>
       <c r="E12" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F12" t="n">
-        <v>15572.36443826622</v>
+        <v>0.5189436797266099</v>
       </c>
       <c r="G12" t="n">
-        <v>299160323.785369</v>
+        <v>0.2886927886325447</v>
       </c>
       <c r="H12" t="n">
-        <v>17296.25172646863</v>
+        <v>0.5373013945938953</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>0: [2119.5520980903393, 19434.42149630692]
-1: [31.492312441329076]</t>
+          <t>0: [0.26583896642435645]</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>0: 200.168278110863
-1: 29.732424755838</t>
+          <t>0: 0.249031371570812</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>11</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>56.667</v>
       </c>
       <c r="E13" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F13" t="n">
-        <v>15566.36443826622</v>
+        <v>0.4961446672112467</v>
       </c>
       <c r="G13" t="n">
-        <v>298973491.4121099</v>
+        <v>0.2742057932852321</v>
       </c>
       <c r="H13" t="n">
-        <v>17290.84993319038</v>
+        <v>0.5236466301669782</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>0: [2547.8966859535035, 23367.878842661783]
-1: [34.49231244132908]</t>
+          <t>0: [0.4253023771396004]</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>0: 241.106090686056
-1: 32.732424755838</t>
+          <t>0: 0.174635935926999</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>12</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>56.667</v>
       </c>
       <c r="E14" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F14" t="n">
-        <v>15560.36443826622</v>
+        <v>0.4745068199723001</v>
       </c>
       <c r="G14" t="n">
-        <v>298786731.0388507</v>
+        <v>0.2651043808285179</v>
       </c>
       <c r="H14" t="n">
-        <v>17285.44853450007</v>
+        <v>0.5148828806908595</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>0: [3015.610344211309, 27663.40891023422]
-1: [37.49231244132908]</t>
+          <t>0: [0.5762653010164671]</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>0: 285.823672335775
-1: 35.732424755838</t>
+          <t>0: 0.104734383994796</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B15" t="n">
         <v>13</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>56.667</v>
       </c>
       <c r="E15" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F15" t="n">
-        <v>15554.36443826622</v>
+        <v>0.4539642175886292</v>
       </c>
       <c r="G15" t="n">
-        <v>298600042.6655915</v>
+        <v>0.260590404051759</v>
       </c>
       <c r="H15" t="n">
-        <v>17280.04753076772</v>
+        <v>0.5104805618745527</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>0: [3522.693072863756, 32321.011699024228]
-1: [40.49231244132908]</t>
+          <t>0: [0.719230984899141]</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0: 334.321023060021
-1: 38.732424755838</t>
+          <t>0: 0.0390331294048891</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B16" t="n">
         <v>14</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>56.667</v>
       </c>
       <c r="E16" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F16" t="n">
-        <v>15548.36443826622</v>
+        <v>0.4344554211915013</v>
       </c>
       <c r="G16" t="n">
-        <v>298413426.2923322</v>
+        <v>0.2599745093411762</v>
       </c>
       <c r="H16" t="n">
-        <v>17274.64692236378</v>
+        <v>0.5098769550991457</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>0: [4069.1448719108444, 37340.68720903181]
-1: [43.49231244132908]</t>
+          <t>0: [0.8546796006293715]</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0: 386.598142858793
-1: 41.732424755838</t>
+          <t>0: -0.0227541751222099</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B17" t="n">
         <v>15</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>56.667</v>
       </c>
       <c r="E17" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F17" t="n">
-        <v>15542.36443826622</v>
+        <v>0.4163457447030774</v>
       </c>
       <c r="G17" t="n">
-        <v>298226881.919073</v>
+        <v>0.2626607275912831</v>
       </c>
       <c r="H17" t="n">
-        <v>17269.24670965914</v>
+        <v>0.5125043683631224</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>0: [4654.965741352574, 42722.43544025696]
-1: [46.49231244132908]</t>
+          <t>0: [0.9830676489984193]</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>0: 442.655031732091
-1: 44.732424755838</t>
+          <t>0: -0.0809003384818603</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B18" t="n">
         <v>16</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="E18" t="n">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="F18" t="n">
-        <v>15536.36443826622</v>
+        <v>0.4091513060877039</v>
       </c>
       <c r="G18" t="n">
-        <v>298040409.5458139</v>
+        <v>0.2681339903900929</v>
       </c>
       <c r="H18" t="n">
-        <v>17263.84689302514</v>
+        <v>0.5178165605599081</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>0: [5280.155681188946, 48466.25639269968]
-1: [49.49231244132908]</t>
+          <t>0: [1.1048272290512375]</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>0: 502.491689679915
-1: 47.732424755838</t>
+          <t>0: -0.135661965413311</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B19" t="n">
         <v>17</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>63.333</v>
       </c>
       <c r="E19" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F19" t="n">
-        <v>15530.36443826622</v>
+        <v>0.4084318075712515</v>
       </c>
       <c r="G19" t="n">
-        <v>297854009.1725547</v>
+        <v>0.2759494862063635</v>
       </c>
       <c r="H19" t="n">
-        <v>17258.44747283355</v>
+        <v>0.5253089435811688</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>0: [5944.714691419959, 54572.15006635998]
-1: [52.49231244132908]</t>
+          <t>0: [1.2203656664712224]</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>0: 566.108116702266
-1: 50.732424755838</t>
+          <t>0: -0.187278563600361</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B20" t="n">
         <v>18</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>63.333</v>
       </c>
       <c r="E20" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F20" t="n">
-        <v>15524.36443826622</v>
+        <v>0.412881640768398</v>
       </c>
       <c r="G20" t="n">
-        <v>297667680.7992955</v>
+        <v>0.2857233903524701</v>
       </c>
       <c r="H20" t="n">
-        <v>17253.04844945656</v>
+        <v>0.534531000366181</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>0: [6648.642772045614, 61040.11646123785]
-1: [55.49231244132908]</t>
+          <t>0: [1.330065594695298]</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>0: 633.504312799143
-1: 53.732424755838</t>
+          <t>0: -0.235972565417688</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B21" t="n">
         <v>19</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>63.333</v>
       </c>
       <c r="E21" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F21" t="n">
-        <v>15518.36443826622</v>
+        <v>0.4220459713037559</v>
       </c>
       <c r="G21" t="n">
-        <v>297481424.4260363</v>
+        <v>0.2971247442364651</v>
       </c>
       <c r="H21" t="n">
-        <v>17247.64982326683</v>
+        <v>0.5450915007927248</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>0: [7391.939923065911, 67870.1555773333]
-1: [58.49231244132908]</t>
+          <t>0: [1.4342854379325427]</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>0: 704.680277970546
-1: 56.732424755838</t>
+          <t>0: -0.281949843529314</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B22" t="n">
         <v>20</v>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>63.333</v>
       </c>
       <c r="E22" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F22" t="n">
-        <v>15512.36443826622</v>
+        <v>0.432674704142043</v>
       </c>
       <c r="G22" t="n">
-        <v>297295240.0527771</v>
+        <v>0.3098683476446034</v>
       </c>
       <c r="H22" t="n">
-        <v>17242.25159463743</v>
+        <v>0.5566581964227271</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>0: [8174.606144480849, 75062.26741464631]
-1: [61.49231244132908]</t>
+          <t>0: [1.533360204556835]</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>0: 779.636012216475
-1: 59.732424755838</t>
+          <t>0: -0.325400497410794</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B23" t="n">
         <v>21</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>63.333</v>
       </c>
       <c r="E23" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F23" t="n">
-        <v>15506.36443826622</v>
+        <v>0.4466382117190685</v>
       </c>
       <c r="G23" t="n">
-        <v>297109127.6795179</v>
+        <v>0.3237085576581287</v>
       </c>
       <c r="H23" t="n">
-        <v>17236.8537639419</v>
+        <v>0.5689539152322697</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>0: [8996.641436290429, 82616.45197317691]
-1: [64.49231244132908]</t>
+          <t>0: [1.6276024987310977]</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>0: 858.371515536931
-1: 62.732424755838</t>
+          <t>0: -0.366499782901654</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B24" t="n">
         <v>22</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>63.333</v>
       </c>
       <c r="E24" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F24" t="n">
-        <v>15500.36443826622</v>
+        <v>0.4611138914418639</v>
       </c>
       <c r="G24" t="n">
-        <v>296923087.3062587</v>
+        <v>0.3384338980322708</v>
       </c>
       <c r="H24" t="n">
-        <v>17231.45633155418</v>
+        <v>0.5817507181192566</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>0: [9858.045798494648, 90532.70925292507]
-1: [67.49231244132908]</t>
+          <t>0: [1.717303671213871]</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>0: 940.886787931913
-1: 65.732424755838</t>
+          <t>0: -0.405409106475281</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B25" t="n">
         <v>23</v>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>66.667</v>
       </c>
       <c r="E25" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F25" t="n">
-        <v>15494.36443826622</v>
+        <v>0.4754648226965509</v>
       </c>
       <c r="G25" t="n">
-        <v>296737118.9329996</v>
+        <v>0.3538623881457308</v>
       </c>
       <c r="H25" t="n">
-        <v>17226.0592978487</v>
+        <v>0.5948633356878963</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>0: [10758.81923109351, 98811.0392538908]
-1: [70.49231244132908]</t>
+          <t>0: [1.802735046436247]</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>0: 1027.18182940142
-1: 68.732424755838</t>
+          <t>0: -0.442277034299206</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B26" t="n">
         <v>24</v>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D26" t="n">
-        <v>0</v>
+        <v>66.667</v>
       </c>
       <c r="E26" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F26" t="n">
-        <v>15488.36443826622</v>
+        <v>0.4900398260711155</v>
       </c>
       <c r="G26" t="n">
-        <v>296551222.5597403</v>
+        <v>0.3698375058355324</v>
       </c>
       <c r="H26" t="n">
-        <v>17220.66266320028</v>
+        <v>0.608142668981163</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>0: [11698.961734087014, 107451.4419760741]
-1: [73.49231244132908]</t>
+          <t>0: [1.884149178061041]</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>0: 1117.25663994546
-1: 71.732424755838</t>
+          <t>0: -0.477240283835213</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B27" t="n">
         <v>25</v>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D27" t="n">
-        <v>0</v>
+        <v>66.667</v>
       </c>
       <c r="E27" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F27" t="n">
-        <v>15482.36443826622</v>
+        <v>0.5057758546879453</v>
       </c>
       <c r="G27" t="n">
-        <v>296365398.1864811</v>
+        <v>0.3862247046709036</v>
       </c>
       <c r="H27" t="n">
-        <v>17215.26642798424</v>
+        <v>0.621469793852367</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>0: [12678.473307475158, 116453.91741947498]
-1: [76.49231244132908]</t>
+          <t>0: [1.9617810980392347]</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>0: 1211.11121956402
-1: 74.732424755838</t>
+          <t>0: -0.510424677432525</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B28" t="n">
         <v>26</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D28" t="n">
-        <v>0</v>
+        <v>66.667</v>
       </c>
       <c r="E28" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F28" t="n">
-        <v>15476.36443826622</v>
+        <v>0.5207646610361444</v>
       </c>
       <c r="G28" t="n">
-        <v>296179645.8132219</v>
+        <v>0.4029084133245072</v>
       </c>
       <c r="H28" t="n">
-        <v>17209.87059257628</v>
+        <v>0.6347506702040631</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>0: [13697.353951257946, 125818.46558409343]
-1: [79.49231244132908]</t>
+          <t>0: [2.0358495344708616]</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>0: 1308.7455682571
-1: 77.732424755838</t>
+          <t>0: -0.541946045399127</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B29" t="n">
         <v>27</v>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D29" t="n">
-        <v>0</v>
+        <v>66.667</v>
       </c>
       <c r="E29" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F29" t="n">
-        <v>15470.36443826622</v>
+        <v>0.5350508562169835</v>
       </c>
       <c r="G29" t="n">
-        <v>295993965.4399627</v>
+        <v>0.4197894521995166</v>
       </c>
       <c r="H29" t="n">
-        <v>17204.4751573526</v>
+        <v>0.6479116083228611</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>0: [14755.603665435376, 135545.08646992946]
-1: [82.49231244132908]</t>
+          <t>0: [2.1065580815905407]</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>0: 1410.15968602472
-1: 80.732424755838</t>
+          <t>0: -0.571911071630114</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B30" t="n">
         <v>28</v>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D30" t="n">
-        <v>0</v>
+        <v>66.667</v>
       </c>
       <c r="E30" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F30" t="n">
-        <v>15464.36443826622</v>
+        <v>0.5486758354050351</v>
       </c>
       <c r="G30" t="n">
-        <v>295808357.0667036</v>
+        <v>0.4367828099304811</v>
       </c>
       <c r="H30" t="n">
-        <v>17199.0801226898</v>
+        <v>0.6608954606671777</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>0: [15853.222450007446, 145633.78007698304]
-1: [85.49231244132908]</t>
+          <t>0: [2.174096311292273]</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>0: 1515.35357286685
-1: 83.732424755838</t>
+          <t>0: -0.600418078764116</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B31" t="n">
         <v>29</v>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D31" t="n">
-        <v>0</v>
+        <v>66.667</v>
       </c>
       <c r="E31" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F31" t="n">
-        <v>15458.36443826622</v>
+        <v>0.5616780282983723</v>
       </c>
       <c r="G31" t="n">
-        <v>295622820.6934443</v>
+        <v>0.4538157294818047</v>
       </c>
       <c r="H31" t="n">
-        <v>17193.68548896496</v>
+        <v>0.6736584664960462</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>0: [16990.210304974156, 156084.5464052542]
-1: [88.49231244132908]</t>
+          <t>0: [2.238640820151586]</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>0: 1624.32722878352
-1: 86.732424755838</t>
+          <t>0: -0.627557752512011</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B32" t="n">
         <v>30</v>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D32" t="n">
-        <v>0</v>
+        <v>66.667</v>
       </c>
       <c r="E32" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F32" t="n">
-        <v>15452.36443826622</v>
+        <v>0.5740931328542932</v>
       </c>
       <c r="G32" t="n">
-        <v>295437356.3201851</v>
+        <v>0.4708260601302683</v>
       </c>
       <c r="H32" t="n">
-        <v>17188.29125655559</v>
+        <v>0.6861676618219984</v>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>0: [18166.567230335506, 166897.3854547429]
-1: [91.49231244132908]</t>
+          <t>0: [2.3003562092244474]</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>0: 1737.08065377471
-1: 89.732424755838</t>
+          <t>0: -0.653413806592809</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B33" t="n">
         <v>31</v>
       </c>
       <c r="C33" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>66.667</v>
       </c>
       <c r="E33" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F33" t="n">
-        <v>15446.36443826622</v>
+        <v>0.5859543322320699</v>
       </c>
       <c r="G33" t="n">
-        <v>295251963.9469259</v>
+        <v>0.48776083754408</v>
       </c>
       <c r="H33" t="n">
-        <v>17182.89742583962</v>
+        <v>0.6983987668546386</v>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>0: [19382.2932260915, 178072.2972254492]
-1: [94.49231244132908]</t>
+          <t>0: [2.3593959962781232]</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>0: 1853.61384784043
-1: 92.732424755838</t>
+          <t>0: -0.678063590863806</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B34" t="n">
         <v>32</v>
       </c>
       <c r="C34" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D34" t="n">
-        <v>0</v>
+        <v>63.333</v>
       </c>
       <c r="E34" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F34" t="n">
-        <v>15440.36443826622</v>
+        <v>0.5972924952986763</v>
       </c>
       <c r="G34" t="n">
-        <v>295066643.5736668</v>
+        <v>0.5045750594345001</v>
       </c>
       <c r="H34" t="n">
-        <v>17177.50399719548</v>
+        <v>0.7103344701156633</v>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>0: [20637.388292242136, 189609.2817173731]
-1: [97.49231244132908]</t>
+          <t>0: [2.415903461763735]</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>0: 1973.92681098067
-1: 95.732424755838</t>
+          <t>0: -0.701578645925393</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B35" t="n">
         <v>33</v>
       </c>
       <c r="C35" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D35" t="n">
-        <v>0</v>
+        <v>63.333</v>
       </c>
       <c r="E35" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F35" t="n">
-        <v>15434.36443826622</v>
+        <v>0.6081363613411589</v>
       </c>
       <c r="G35" t="n">
-        <v>294881395.2004076</v>
+        <v>0.5212306288742631</v>
       </c>
       <c r="H35" t="n">
-        <v>17172.11097100201</v>
+        <v>0.7219630384405168</v>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>0: [21931.852428787417, 201508.33893051452]
-1: [100.49231244132908]</t>
+          <t>0: [2.4700124309520035]</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>0: 2098.01954319544
-1: 98.732424755838</t>
+          <t>0: -0.724025207848315</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B36" t="n">
         <v>34</v>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D36" t="n">
-        <v>0</v>
+        <v>63.333</v>
       </c>
       <c r="E36" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F36" t="n">
-        <v>15428.36443826622</v>
+        <v>0.6185127098089687</v>
       </c>
       <c r="G36" t="n">
-        <v>294696218.8271484</v>
+        <v>0.5376954413920706</v>
       </c>
       <c r="H36" t="n">
-        <v>17166.7183476385</v>
+        <v>0.7332771927396015</v>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>0: [23265.685635727335, 213769.46886487352]
-1: [103.49231244132908]</t>
+          <t>0: [2.521847995361693]</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>0: 2225.89204448474
-1: 101.732424755838</t>
+          <t>0: -0.745464666811013</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B37" t="n">
         <v>35</v>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D37" t="n">
-        <v>0</v>
+        <v>63.333</v>
       </c>
       <c r="E37" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F37" t="n">
-        <v>15422.36443826622</v>
+        <v>0.6284465160107641</v>
       </c>
       <c r="G37" t="n">
-        <v>294511114.4538892</v>
+        <v>0.5539425954194269</v>
       </c>
       <c r="H37" t="n">
-        <v>17161.32612748471</v>
+        <v>0.7442731994499244</v>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>0: [24638.887913061895, 226392.6715204501]
-1: [106.49231244132908]</t>
+          <t>0: [2.57152717702218]</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>0: 2357.54431484856
-1: 104.732424755838</t>
+          <t>0: -0.765953983419294</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B38" t="n">
         <v>36</v>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D38" t="n">
-        <v>0</v>
+        <v>63.333</v>
       </c>
       <c r="E38" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F38" t="n">
-        <v>15416.36443826622</v>
+        <v>0.6379610937353071</v>
       </c>
       <c r="G38" t="n">
-        <v>294326082.08063</v>
+        <v>0.5699497086447255</v>
       </c>
       <c r="H38" t="n">
-        <v>17155.93431092081</v>
+        <v>0.754950136528715</v>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>0: [26051.459260791096, 239377.94689724426]
-1: [109.49231244132908]</t>
+          <t>0: [2.6191595393094307]</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>0: 2492.97635428691
-1: 107.732424755838</t>
+          <t>0: -0.785546066362641</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B39" t="n">
         <v>37</v>
       </c>
       <c r="C39" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D39" t="n">
-        <v>0</v>
+        <v>63.333</v>
       </c>
       <c r="E39" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F39" t="n">
-        <v>15410.36443826622</v>
+        <v>0.6470782257719238</v>
       </c>
       <c r="G39" t="n">
-        <v>294141121.7073708</v>
+        <v>0.5856983253791177</v>
       </c>
       <c r="H39" t="n">
-        <v>17150.54289832747</v>
+        <v>0.7653093004655815</v>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>0: [27503.399678914942, 252725.294995256]
-1: [112.49231244132908]</t>
+          <t>0: [2.6648477481405846]</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>0: 2632.18816279979
-1: 110.732424755838</t>
+          <t>0: -0.804290114879149</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B40" t="n">
         <v>38</v>
       </c>
       <c r="C40" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D40" t="n">
-        <v>0</v>
+        <v>63.333</v>
       </c>
       <c r="E40" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F40" t="n">
-        <v>15404.36443826622</v>
+        <v>0.6558182832850774</v>
       </c>
       <c r="G40" t="n">
-        <v>293956233.3341116</v>
+        <v>0.6011734022153273</v>
       </c>
       <c r="H40" t="n">
-        <v>17145.15189008577</v>
+        <v>0.7753537271564039</v>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>0: [28994.709167433426, 266434.71581448533]
-1: [115.49231244132908]</t>
+          <t>0: [2.70868808725308]</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>0: 2775.17974038719
-1: 113.732424755838</t>
+          <t>0: -0.822231929281554</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B41" t="n">
         <v>39</v>
       </c>
       <c r="C41" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D41" t="n">
-        <v>0</v>
+        <v>63.333</v>
       </c>
       <c r="E41" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F41" t="n">
-        <v>15398.36443826622</v>
+        <v>0.6642003349591329</v>
       </c>
       <c r="G41" t="n">
-        <v>293771416.9608524</v>
+        <v>0.6163628611154299</v>
       </c>
       <c r="H41" t="n">
-        <v>17139.76128657725</v>
+        <v>0.7850878047170456</v>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>0: [30525.387726346555, 280506.20935493225]
-1: [118.49231244132908]</t>
+          <t>0: [2.750770931164407]</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>0: 2921.95108704912
-1: 116.732424755838</t>
+          <t>0: -0.839414192559148</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B42" t="n">
         <v>40</v>
       </c>
       <c r="C42" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D42" t="n">
-        <v>0</v>
+        <v>63.333</v>
       </c>
       <c r="E42" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F42" t="n">
-        <v>15392.36443826622</v>
+        <v>0.6722422467800507</v>
       </c>
       <c r="G42" t="n">
-        <v>293586672.5875932</v>
+        <v>0.6312572006424232</v>
       </c>
       <c r="H42" t="n">
-        <v>17134.37108818393</v>
+        <v>0.7945169605756841</v>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>0: [32095.435355654325, 294939.77561659674]
-1: [121.49231244132908]</t>
+          <t>0: [2.791181179233704]</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>0: 3072.50220278557
-1: 119.732424755838</t>
+          <t>0: -0.855876725827773</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B43" t="n">
         <v>41</v>
       </c>
       <c r="C43" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D43" t="n">
-        <v>0</v>
+        <v>63.333</v>
       </c>
       <c r="E43" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F43" t="n">
-        <v>15386.36443826622</v>
+        <v>0.6799607732654034</v>
       </c>
       <c r="G43" t="n">
-        <v>293402000.214334</v>
+        <v>0.6458491573934659</v>
       </c>
       <c r="H43" t="n">
-        <v>17128.98129528823</v>
+        <v>0.8036474086273568</v>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>0: [33704.852055356736, 309735.41459947877]
-1: [124.49231244132908]</t>
+          <t>0: [2.8299986540451543]</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>0: 3226.83308759655
-1: 122.732424755838</t>
+          <t>0: -0.871656720161362</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B44" t="n">
         <v>42</v>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D44" t="n">
-        <v>0</v>
+        <v>63.333</v>
       </c>
       <c r="E44" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F44" t="n">
-        <v>15380.36443826622</v>
+        <v>0.6873716408961532</v>
       </c>
       <c r="G44" t="n">
-        <v>293217399.8410748</v>
+        <v>0.6601334108349063</v>
       </c>
       <c r="H44" t="n">
-        <v>17123.59190827307</v>
+        <v>0.8124859450076083</v>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>0: [35353.63782545379, 324893.1263035784]
-1: [127.49231244132908]</t>
+          <t>0: [2.8672984671189585]</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>0: 3384.94374148206
-1: 125.732424755838</t>
+          <t>0: -0.886788947109361</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B45" t="n">
         <v>43</v>
       </c>
       <c r="C45" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D45" t="n">
-        <v>0</v>
+        <v>63.333</v>
       </c>
       <c r="E45" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F45" t="n">
-        <v>15374.36443826622</v>
+        <v>0.6944896244454474</v>
       </c>
       <c r="G45" t="n">
-        <v>293032871.4678156</v>
+        <v>0.6741063257108458</v>
       </c>
       <c r="H45" t="n">
-        <v>17118.20292752179</v>
+        <v>0.8210397832692675</v>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>0: [37041.79266594549, 340412.9107288956]
-1: [130.4923124413291]</t>
+          <t>0: [2.903151354737721]</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>0: 3546.83416444209
-1: 128.732424755838</t>
+          <t>0: -0.901305949988265</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B46" t="n">
         <v>44</v>
       </c>
       <c r="C46" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D46" t="n">
-        <v>0</v>
+        <v>63.333</v>
       </c>
       <c r="E46" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F46" t="n">
-        <v>15368.36443826622</v>
+        <v>0.7013286168428911</v>
       </c>
       <c r="G46" t="n">
-        <v>292848415.0945564</v>
+        <v>0.6877657270238402</v>
       </c>
       <c r="H46" t="n">
-        <v>17112.81435341821</v>
+        <v>0.8293164215327224</v>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>0: [38769.31657683182, 356294.76787543035]
-1: [133.4923124413291]</t>
+          <t>0: [2.9376239864613427]</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>0: 3712.50435647665
-1: 131.732424755838</t>
+          <t>0: -0.915238217834343</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B47" t="n">
         <v>45</v>
       </c>
       <c r="C47" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D47" t="n">
-        <v>0</v>
+        <v>63.333</v>
       </c>
       <c r="E47" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F47" t="n">
-        <v>15362.36443826622</v>
+        <v>0.7079016931583818</v>
       </c>
       <c r="G47" t="n">
-        <v>292664030.7212972</v>
+        <v>0.7011107032904379</v>
       </c>
       <c r="H47" t="n">
-        <v>17107.42618634659</v>
+        <v>0.8373235356123927</v>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>0: [40536.209558112794, 372538.6977431827]
-1: [136.4923124413291]</t>
+          <t>0: [2.970779248695932]</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>0: 3881.95431758574
-1: 134.732424755838</t>
+          <t>0: -0.928614343719175</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B48" t="n">
         <v>46</v>
       </c>
       <c r="C48" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D48" t="n">
-        <v>0</v>
+        <v>63.333</v>
       </c>
       <c r="E48" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F48" t="n">
-        <v>15356.36443826622</v>
+        <v>0.7142211692382714</v>
       </c>
       <c r="G48" t="n">
-        <v>292479718.348038</v>
+        <v>0.714141434374348</v>
       </c>
       <c r="H48" t="n">
-        <v>17102.03842669166</v>
+        <v>0.8450688932710445</v>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>0: [42342.47160978841, 389144.7003321526]
-1: [139.4923124413291]</t>
+          <t>0: [3.0026765054848648]</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>0: 4055.18404776935
-1: 137.732424755838</t>
+          <t>0: -0.941461168959939</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B49" t="n">
         <v>47</v>
       </c>
       <c r="C49" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D49" t="n">
-        <v>0</v>
+        <v>63.333</v>
       </c>
       <c r="E49" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F49" t="n">
-        <v>15350.36443826622</v>
+        <v>0.7202986554787081</v>
       </c>
       <c r="G49" t="n">
-        <v>292295477.9747788</v>
+        <v>0.7268590407119567</v>
       </c>
       <c r="H49" t="n">
-        <v>17096.65107483857</v>
+        <v>0.8525602856760082</v>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>0: [44188.102731858664, 406112.7756423401]
-1: [142.4923124413291]</t>
+          <t>0: [3.0333718385044746]</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>0: 4232.19354702748
-1: 140.732424755838</t>
+          <t>0: -0.953803914602011</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B50" t="n">
         <v>48</v>
       </c>
       <c r="C50" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D50" t="n">
-        <v>0</v>
+        <v>63.333</v>
       </c>
       <c r="E50" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F50" t="n">
-        <v>15344.36443826622</v>
+        <v>0.726145106176637</v>
       </c>
       <c r="G50" t="n">
-        <v>292111309.6015196</v>
+        <v>0.7392654511821429</v>
       </c>
       <c r="H50" t="n">
-        <v>17091.26413117297</v>
+        <v>0.8598054728728719</v>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>0: [46073.10292432357, 423442.9236737451]
-1: [145.4923124413291]</t>
+          <t>0: [3.0629182680737834]</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>0: 4412.98281536015
-1: 143.732424755838</t>
+          <t>0: -0.965666301411611</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B51" t="n">
         <v>49</v>
       </c>
       <c r="C51" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D51" t="n">
-        <v>0</v>
+        <v>63.333</v>
       </c>
       <c r="E51" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F51" t="n">
-        <v>15338.36443826622</v>
+        <v>0.7317708648581098</v>
       </c>
       <c r="G51" t="n">
-        <v>291927213.2282605</v>
+        <v>0.7513632872461796</v>
       </c>
       <c r="H51" t="n">
-        <v>17085.87759608094</v>
+        <v>0.866812140689192</v>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>0: [47997.47218718311, 441135.14442636777]
-1: [148.4923124413291]</t>
+          <t>0: [3.0913659568274086]</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>0: 4597.55185276734
-1: 146.732424755838</t>
+          <t>0: -0.977070659490041</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B52" t="n">
         <v>50</v>
       </c>
       <c r="C52" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D52" t="n">
-        <v>0</v>
+        <v>63.333</v>
       </c>
       <c r="E52" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F52" t="n">
-        <v>15332.36443826622</v>
+        <v>0.7371857059461574</v>
       </c>
       <c r="G52" t="n">
-        <v>291743188.8550013</v>
+        <v>0.7631557613035915</v>
       </c>
       <c r="H52" t="n">
-        <v>17080.49146994902</v>
+        <v>0.8735878669622144</v>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>0: [49961.2105204373, 459189.43790020794]
-1: [151.4923124413291]</t>
+          <t>0: [3.118762397553141]</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>0: 4785.90065924906
-1: 149.732424755838</t>
+          <t>0: -0.988038028507472</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B53" t="n">
         <v>51</v>
       </c>
       <c r="C53" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D53" t="n">
-        <v>0</v>
+        <v>63.333</v>
       </c>
       <c r="E53" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F53" t="n">
-        <v>15326.36443826622</v>
+        <v>0.7423988730963834</v>
       </c>
       <c r="G53" t="n">
-        <v>291559236.4817421</v>
+        <v>0.7746465874842298</v>
       </c>
       <c r="H53" t="n">
-        <v>17075.10575316423</v>
+        <v>0.8801400953735887</v>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>0: [51964.31792408613, 477605.8040952657]
-1: [154.4923124413291]</t>
+          <t>0: [3.145152586560259]</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>0: 4978.0292348053
-1: 152.732424755838</t>
+          <t>0: -0.998588249452177</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B54" t="n">
         <v>52</v>
       </c>
       <c r="C54" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D54" t="n">
-        <v>0</v>
+        <v>63.333</v>
       </c>
       <c r="E54" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F54" t="n">
-        <v>15320.36443826622</v>
+        <v>0.7474191144974166</v>
       </c>
       <c r="G54" t="n">
-        <v>291375356.1084829</v>
+        <v>0.7858399033323792</v>
       </c>
       <c r="H54" t="n">
-        <v>17069.72044611402</v>
+        <v>0.8864761154889506</v>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>0: [54006.7943981296, 496384.243011541]
-1: [157.4923124413291]</t>
+          <t>0: [3.170579183820807]</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>0: 5173.93757943607
-1: 155.732424755838</t>
+          <t>0: -1.00874004869963</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B55" t="n">
         <v>53</v>
       </c>
       <c r="C55" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D55" t="n">
-        <v>0</v>
+        <v>63.333</v>
       </c>
       <c r="E55" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F55" t="n">
-        <v>15314.36443826622</v>
+        <v>0.752254715405227</v>
       </c>
       <c r="G55" t="n">
-        <v>291191547.7352237</v>
+        <v>0.7967402010412096</v>
       </c>
       <c r="H55" t="n">
-        <v>17064.33554918631</v>
+        <v>0.8926030478556577</v>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>0: [56088.63994256771, 515524.75464903394]
-1: [160.4923124413291]</t>
+          <t>0: [3.195082661013131]</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>0: 5373.62569314136
-1: 158.732424755838</t>
+          <t>0: -1.0185111151239</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B56" t="n">
         <v>54</v>
       </c>
       <c r="C56" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D56" t="n">
-        <v>0</v>
+        <v>63.333</v>
       </c>
       <c r="E56" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F56" t="n">
-        <v>15308.36443826622</v>
+        <v>0.7569135281548327</v>
       </c>
       <c r="G56" t="n">
-        <v>291007811.3619645</v>
+        <v>0.8073522670702098</v>
       </c>
       <c r="H56" t="n">
-        <v>17058.95106276949</v>
+        <v>0.8985278332195447</v>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>0: [58209.85455740046, 535027.3390077443]
-1: [163.4923124413291]</t>
+          <t>0: [3.218701438494195]</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>0: 5577.09357592118
-1: 161.732424755838</t>
+          <t>0: -1.02791817090028</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B57" t="n">
         <v>55</v>
       </c>
       <c r="C57" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D57" t="n">
-        <v>0</v>
+        <v>63.333</v>
       </c>
       <c r="E57" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F57" t="n">
-        <v>15302.36443826622</v>
+        <v>0.7614029998698818</v>
       </c>
       <c r="G57" t="n">
-        <v>290824146.9887053</v>
+        <v>0.817681129128518</v>
       </c>
       <c r="H57" t="n">
-        <v>17053.56698725241</v>
+        <v>0.9042572250905812</v>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>0: [60370.43824262785, 554891.9960876723]
-1: [166.4923124413291]</t>
+          <t>0: [3.2414720121337472]</t>
         </is>
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>0: 5784.34122777553
-1: 164.732424755838</t>
+          <t>0: -1.03697703658274</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B58" t="n">
         <v>56</v>
       </c>
       <c r="C58" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D58" t="n">
-        <v>0</v>
+        <v>63.333</v>
       </c>
       <c r="E58" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F58" t="n">
-        <v>15296.36443826622</v>
+        <v>0.7657301980697852</v>
       </c>
       <c r="G58" t="n">
-        <v>290640554.6154461</v>
+        <v>0.827732009636816</v>
       </c>
       <c r="H58" t="n">
-        <v>17048.18332302436</v>
+        <v>0.9097977850252308</v>
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>0: [62570.39099824988, 575118.7258888179]
-1: [169.4923124413291]</t>
+          <t>0: [3.2634290708586997]</t>
         </is>
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>0: 5995.3686487044
-1: 167.732424755838</t>
+          <t>0: -1.04570269098066</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B59" t="n">
         <v>57</v>
       </c>
       <c r="C59" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D59" t="n">
-        <v>0</v>
+        <v>63.333</v>
       </c>
       <c r="E59" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F59" t="n">
-        <v>15290.36443826622</v>
+        <v>0.7699018343552885</v>
       </c>
       <c r="G59" t="n">
-        <v>290457034.2421869</v>
+        <v>0.8375102848926272</v>
       </c>
       <c r="H59" t="n">
-        <v>17042.80007047512</v>
+        <v>0.9151558801060218</v>
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>0: [64809.71282426656, 595707.5284111811]
-1: [172.4923124413291]</t>
+          <t>0: [3.284605605679143]</t>
         </is>
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>0: 6210.1758387078
-1: 170.732424755838</t>
+          <t>0: -1.05410932630712</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B60" t="n">
         <v>58</v>
       </c>
       <c r="C60" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D60" t="n">
-        <v>0</v>
+        <v>66.667</v>
       </c>
       <c r="E60" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F60" t="n">
-        <v>15284.36443826622</v>
+        <v>0.7739335255578492</v>
       </c>
       <c r="G60" t="n">
-        <v>290273585.8689277</v>
+        <v>0.8470214492609736</v>
       </c>
       <c r="H60" t="n">
-        <v>17037.41722999492</v>
+        <v>0.9203376821911474</v>
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>0: [67088.40372067787, 616658.4036547618]
-1: [175.4923124413291]</t>
+          <t>0: [3.305033010897767]</t>
         </is>
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>0: 6428.76279778573
-1: 173.732424755838</t>
+          <t>0: -1.06221039902402</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B61" t="n">
         <v>59</v>
       </c>
       <c r="C61" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D61" t="n">
-        <v>0</v>
+        <v>66.667</v>
       </c>
       <c r="E61" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F61" t="n">
-        <v>15278.36443826622</v>
+        <v>0.777921621329296</v>
       </c>
       <c r="G61" t="n">
-        <v>290090209.4956685</v>
+        <v>0.856271083796554</v>
       </c>
       <c r="H61" t="n">
-        <v>17032.03480197444</v>
+        <v>0.9253491685826243</v>
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>0: [69406.46368748385, 637971.3516195602]
-1: [178.4923124413291]</t>
+          <t>0: [3.3247411781413545]</t>
         </is>
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>0: 6651.12952593818
-1: 176.732424755838</t>
+          <t>0: -1.07001867676707</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B62" t="n">
         <v>60</v>
       </c>
       <c r="C62" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D62" t="n">
-        <v>0</v>
+        <v>66.667</v>
       </c>
       <c r="E62" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F62" t="n">
-        <v>15272.36443826622</v>
+        <v>0.7817681130136823</v>
       </c>
       <c r="G62" t="n">
-        <v>289906905.1224093</v>
+        <v>0.8652648287767268</v>
       </c>
       <c r="H62" t="n">
-        <v>17026.65278680485</v>
+        <v>0.9301961238237487</v>
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>0: [71763.89272468444, 659646.3723055761]
-1: [181.4923124413291]</t>
+          <t>0: [3.3437585837958332]</t>
         </is>
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>0: 6877.27602316516
-1: 179.732424755838</t>
+          <t>0: -1.07754628169644</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B63" t="n">
         <v>61</v>
       </c>
       <c r="C63" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D63" t="n">
-        <v>0</v>
+        <v>66.667</v>
       </c>
       <c r="E63" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F63" t="n">
-        <v>15266.36443826622</v>
+        <v>0.7854786905767528</v>
       </c>
       <c r="G63" t="n">
-        <v>289723672.7491502</v>
+        <v>0.8740083596881253</v>
       </c>
       <c r="H63" t="n">
-        <v>17021.27118487777</v>
+        <v>0.9348841423877748</v>
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>0: [74160.6908322797, 681683.4657128096]
-1: [184.4923124413291]</t>
+          <t>0: [3.3621123703746125]</t>
         </is>
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>0: 7107.20228946667
-1: 182.732424755838</t>
+          <t>0: -1.08480473058495</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B64" t="n">
         <v>62</v>
       </c>
       <c r="C64" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D64" t="n">
-        <v>0</v>
+        <v>66.667</v>
       </c>
       <c r="E64" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F64" t="n">
-        <v>15260.36443826622</v>
+        <v>0.7890587714914912</v>
       </c>
       <c r="G64" t="n">
-        <v>289540512.375891</v>
+        <v>0.8825073662651017</v>
       </c>
       <c r="H64" t="n">
-        <v>17015.88999658528</v>
+        <v>0.9394186320619268</v>
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>0: [76596.85801026957, 704082.6318412607]
-1: [187.4923124413291]</t>
+          <t>0: [3.3798284223030577]</t>
         </is>
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>0: 7340.9083248427
-1: 185.732424755838</t>
+          <t>0: -1.09180497192568</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B65" t="n">
         <v>63</v>
       </c>
       <c r="C65" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D65" t="n">
-        <v>0</v>
+        <v>66.667</v>
       </c>
       <c r="E65" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F65" t="n">
-        <v>15254.36443826622</v>
+        <v>0.7925135166548297</v>
       </c>
       <c r="G65" t="n">
-        <v>289357424.0026317</v>
+        <v>0.8907675342264157</v>
       </c>
       <c r="H65" t="n">
-        <v>17010.50922231994</v>
+        <v>0.9438048178656516</v>
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>0: [79072.3942586541, 726843.8706909294]
-1: [190.4923124413291]</t>
+          <t>0: [3.396931436559476]</t>
         </is>
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>0: 7578.39412929326
-1: 188.732424755838</t>
+          <t>0: -1.09855742031392</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B66" t="n">
         <v>64</v>
       </c>
       <c r="C66" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D66" t="n">
-        <v>0</v>
+        <v>66.667</v>
       </c>
       <c r="E66" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F66" t="n">
-        <v>15248.36443826622</v>
+        <v>0.7958478451904619</v>
       </c>
       <c r="G66" t="n">
-        <v>289174407.6293725</v>
+        <v>0.8987945293987265</v>
       </c>
       <c r="H66" t="n">
-        <v>17005.12886247477</v>
+        <v>0.9480477463707861</v>
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>0: [81587.29957743327, 749967.1822618155]
-1: [193.4923124413291]</t>
+          <t>0: [3.4134449885745415]</t>
         </is>
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>0: 7819.65970281834
-1: 191.732424755838</t>
+          <t>0: -1.10507198833393</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B67" t="n">
         <v>65</v>
       </c>
       <c r="C67" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D67" t="n">
-        <v>0</v>
+        <v>66.667</v>
       </c>
       <c r="E67" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F67" t="n">
-        <v>15242.36443826622</v>
+        <v>0.7990664482277037</v>
       </c>
       <c r="G67" t="n">
-        <v>288991463.2561134</v>
+        <v>0.906593983952241</v>
       </c>
       <c r="H67" t="n">
-        <v>16999.74891744326</v>
+        <v>0.952152290315074</v>
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>0: [84141.57396660706, 773452.5665539192]
-1: [196.4923124413291]</t>
+          <t>0: [3.4293915937561867]</t>
         </is>
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>0: 8064.70504541795
-1: 194.732424755838</t>
+          <t>0: -1.1113581161596</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B68" t="n">
         <v>66</v>
       </c>
       <c r="C68" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D68" t="n">
-        <v>0</v>
+        <v>66.667</v>
       </c>
       <c r="E68" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F68" t="n">
-        <v>15236.36443826622</v>
+        <v>0.8021738017382594</v>
       </c>
       <c r="G68" t="n">
-        <v>288808590.8828542</v>
+        <v>0.9141714845060968</v>
       </c>
       <c r="H68" t="n">
-        <v>16994.36938761936</v>
+        <v>0.9561231534201526</v>
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>0: [86735.21742617551, 797300.0235672406]
-1: [199.4923124413291]</t>
+          <t>0: [3.4447927649754093]</t>
         </is>
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>0: 8313.53015709209
-1: 197.732424755838</t>
+          <t>0: -1.11742479905838</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B69" t="n">
         <v>67</v>
       </c>
       <c r="C69" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D69" t="n">
-        <v>0</v>
+        <v>66.667</v>
       </c>
       <c r="E69" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F69" t="n">
-        <v>15230.36443826622</v>
+        <v>0.8051741785054489</v>
       </c>
       <c r="G69" t="n">
-        <v>288625790.509595</v>
+        <v>0.921532561889299</v>
       </c>
       <c r="H69" t="n">
-        <v>16988.9902733975</v>
+        <v>0.9599648753414362</v>
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>0: [89368.2299561386, 821509.5533017794]
-1: [202.4923124413291]</t>
+          <t>0: [3.4596690663197562]</t>
         </is>
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>0: 8566.13503784075
-1: 200.732424755838</t>
+          <t>0: -1.12328061297028</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B70" t="n">
         <v>68</v>
       </c>
       <c r="C70" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="D70" t="n">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="E70" t="n">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="F70" t="n">
-        <v>15224.36443826622</v>
+        <v>0.8080876457350807</v>
       </c>
       <c r="G70" t="n">
-        <v>288443062.1363358</v>
+        <v>0.9286826823677836</v>
       </c>
       <c r="H70" t="n">
-        <v>16983.61157517257</v>
+        <v>0.9636818366908155</v>
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>0: [92040.61155649634, 846081.155757536]
-1: [205.4923124413291]</t>
+          <t>0: [3.4740401633952125]</t>
         </is>
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>0: 8822.51968766394
-1: 203.732424755838</t>
+          <t>0: -1.12893373831813</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>EmptyModel_All_Default</t>
+          <t>BCEWL_LR_Set_to_point1</t>
         </is>
       </c>
       <c r="B71" t="n">
         <v>69</v>
       </c>
       <c r="C71" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="D71" t="n">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="E71" t="n">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="F71" t="n">
-        <v>15218.36443826622</v>
+        <v>0.8109389410832962</v>
       </c>
       <c r="G71" t="n">
-        <v>288260405.7630765</v>
+        <v>0.9356272401699518</v>
       </c>
       <c r="H71" t="n">
-        <v>16978.23329333993</v>
+        <v>0.9672782640843077</v>
       </c>
       <c r="I71" t="inlineStr">
         <is>
-          <t>0: [94752.36222724871, 871014.83093451]
-1: [208.4923124413291]</t>
+          <t>0: [3.4879248704336328]</t>
         </is>
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>0: 9082.68410656165
-1: 206.732424755838</t>
+          <t>0: -1.13439198219108</t>
         </is>
       </c>
     </row>

</xml_diff>